<commit_message>
Try and fail to improve tri()
</commit_message>
<xml_diff>
--- a/ivtools/sampledata/CeRAM_Depositions.xlsx
+++ b/ivtools/sampledata/CeRAM_Depositions.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\emrl\Pool\Projekte\HGST-CERAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="12045"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="deposition_plan" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="249">
   <si>
     <t>wafer_number</t>
   </si>
@@ -643,9 +643,6 @@
     <t>JR576</t>
   </si>
   <si>
-    <t>Beamline 5 nm amorphous</t>
-  </si>
-  <si>
     <t>Beamline 10 nm amorphous (initally forgot Ta protection layer)</t>
   </si>
   <si>
@@ -698,12 +695,84 @@
   </si>
   <si>
     <t>Reh</t>
+  </si>
+  <si>
+    <t>AH1</t>
+  </si>
+  <si>
+    <t>Ahorn</t>
+  </si>
+  <si>
+    <t>NiO</t>
+  </si>
+  <si>
+    <t>NiO first test</t>
+  </si>
+  <si>
+    <t>Ahorn2</t>
+  </si>
+  <si>
+    <t>LAMA1</t>
+  </si>
+  <si>
+    <t>Lama</t>
+  </si>
+  <si>
+    <t>TE thickness variation</t>
+  </si>
+  <si>
+    <t>LAMA2</t>
+  </si>
+  <si>
+    <t>LAMA3</t>
+  </si>
+  <si>
+    <t>LAMA4</t>
+  </si>
+  <si>
+    <t>Beamline 5 nm amorphous, Pt added 2019-04-23</t>
+  </si>
+  <si>
+    <t>Beamline 5 nm crystalline, Pt added 2019-04-23</t>
+  </si>
+  <si>
+    <t>Pferd1</t>
+  </si>
+  <si>
+    <t>Pferd</t>
+  </si>
+  <si>
+    <t>Pferd2</t>
+  </si>
+  <si>
+    <t>amorphous</t>
+  </si>
+  <si>
+    <t>crystalline</t>
+  </si>
+  <si>
+    <t>Pferd3</t>
+  </si>
+  <si>
+    <t>crystalline w/ high O2</t>
+  </si>
+  <si>
+    <t>Dachs1</t>
+  </si>
+  <si>
+    <t>Dachs</t>
+  </si>
+  <si>
+    <t>contact test</t>
+  </si>
+  <si>
+    <t>TE thickness variation, additional 60nm Pt added 2019-04-26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1325,7 +1394,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1400,50 +1469,57 @@
     <xf numFmtId="0" fontId="0" fillId="55" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="47" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="49" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="52" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1726,14 +1802,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T117"/>
+  <dimension ref="A1:T127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H104" sqref="H104"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M123" sqref="M123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -1787,7 +1863,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -6281,7 +6357,7 @@
       </c>
       <c r="S95" s="43"/>
       <c r="T95" s="43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
@@ -6335,7 +6411,7 @@
       </c>
       <c r="S96" s="43"/>
       <c r="T96" s="43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
@@ -6389,7 +6465,7 @@
       </c>
       <c r="S97" s="43"/>
       <c r="T97" s="43" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="98" spans="1:20" x14ac:dyDescent="0.25">
@@ -6496,7 +6572,7 @@
       </c>
       <c r="S99" s="55"/>
       <c r="T99" s="54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="100" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.25">
@@ -6549,7 +6625,7 @@
       </c>
       <c r="S100" s="55"/>
       <c r="T100" s="54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="101" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.25">
@@ -6602,7 +6678,7 @@
       </c>
       <c r="S101" s="55"/>
       <c r="T101" s="54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="102" spans="1:20" x14ac:dyDescent="0.25">
@@ -6710,7 +6786,7 @@
       </c>
       <c r="S103" s="59"/>
       <c r="T103" s="58" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="104" spans="1:20" x14ac:dyDescent="0.25">
@@ -6818,7 +6894,7 @@
       </c>
       <c r="S105" s="59"/>
       <c r="T105" s="58" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
     </row>
     <row r="106" spans="1:20" x14ac:dyDescent="0.25">
@@ -6872,7 +6948,7 @@
       </c>
       <c r="S106" s="59"/>
       <c r="T106" s="58" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
     </row>
     <row r="107" spans="1:20" x14ac:dyDescent="0.25">
@@ -6926,7 +7002,7 @@
       </c>
       <c r="S107" s="59"/>
       <c r="T107" s="58" t="s">
-        <v>207</v>
+        <v>236</v>
       </c>
     </row>
     <row r="108" spans="1:20" x14ac:dyDescent="0.25">
@@ -6941,7 +7017,7 @@
         <v>43311</v>
       </c>
       <c r="E108" s="58" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F108" s="56" t="s">
         <v>181</v>
@@ -6980,7 +7056,7 @@
       </c>
       <c r="S108" s="59"/>
       <c r="T108" s="58" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
     </row>
     <row r="109" spans="1:20" x14ac:dyDescent="0.25">
@@ -6995,7 +7071,7 @@
         <v>43311</v>
       </c>
       <c r="E109" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F109" s="56" t="s">
         <v>181</v>
@@ -7034,7 +7110,7 @@
       </c>
       <c r="S109" s="59"/>
       <c r="T109" s="58" t="s">
-        <v>212</v>
+        <v>237</v>
       </c>
     </row>
     <row r="110" spans="1:20" x14ac:dyDescent="0.25">
@@ -7049,7 +7125,7 @@
         <v>43311</v>
       </c>
       <c r="E110" s="58" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F110" s="56" t="s">
         <v>181</v>
@@ -7088,7 +7164,7 @@
       </c>
       <c r="S110" s="59"/>
       <c r="T110" s="58" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:20" x14ac:dyDescent="0.25">
@@ -7103,7 +7179,7 @@
         <v>43313</v>
       </c>
       <c r="E111" s="58" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F111" s="56" t="s">
         <v>181</v>
@@ -7142,7 +7218,7 @@
       </c>
       <c r="S111" s="59"/>
       <c r="T111" s="58" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="112" spans="1:20" x14ac:dyDescent="0.25">
@@ -7157,7 +7233,7 @@
         <v>43314</v>
       </c>
       <c r="E112" s="58" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F112" s="56" t="s">
         <v>181</v>
@@ -7196,7 +7272,7 @@
       </c>
       <c r="S112" s="59"/>
       <c r="T112" s="58" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
@@ -7211,7 +7287,7 @@
         <v>43314</v>
       </c>
       <c r="E113" s="58" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F113" s="56" t="s">
         <v>181</v>
@@ -7250,7 +7326,7 @@
       </c>
       <c r="S113" s="59"/>
       <c r="T113" s="58" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
@@ -7265,10 +7341,10 @@
         <v>43420</v>
       </c>
       <c r="E114" s="62" t="s">
+        <v>217</v>
+      </c>
+      <c r="F114" s="60" t="s">
         <v>218</v>
-      </c>
-      <c r="F114" s="60" t="s">
-        <v>219</v>
       </c>
       <c r="G114" s="63">
         <v>1</v>
@@ -7298,7 +7374,7 @@
       <c r="R114" s="63"/>
       <c r="S114" s="63"/>
       <c r="T114" s="62" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.25">
@@ -7311,10 +7387,10 @@
         <v>43493</v>
       </c>
       <c r="E115" s="64" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F115" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G115" s="65">
         <v>1</v>
@@ -7346,7 +7422,7 @@
       <c r="R115" s="65"/>
       <c r="S115" s="65"/>
       <c r="T115" s="34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.25">
@@ -7359,10 +7435,10 @@
         <v>43493</v>
       </c>
       <c r="E116" s="64" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F116" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G116" s="65">
         <v>2</v>
@@ -7394,7 +7470,7 @@
       <c r="R116" s="65"/>
       <c r="S116" s="65"/>
       <c r="T116" s="34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.25">
@@ -7407,10 +7483,10 @@
         <v>43493</v>
       </c>
       <c r="E117" s="64" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F117" s="34" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G117" s="65">
         <v>3</v>
@@ -7442,7 +7518,475 @@
       <c r="R117" s="65"/>
       <c r="S117" s="65"/>
       <c r="T117" s="34" t="s">
-        <v>224</v>
+        <v>223</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A118" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B118" s="66"/>
+      <c r="C118" s="66"/>
+      <c r="D118" s="67">
+        <v>43538</v>
+      </c>
+      <c r="E118" s="68" t="s">
+        <v>225</v>
+      </c>
+      <c r="F118" s="66" t="s">
+        <v>226</v>
+      </c>
+      <c r="G118" s="69">
+        <v>1</v>
+      </c>
+      <c r="H118" s="66"/>
+      <c r="I118" s="68" t="s">
+        <v>227</v>
+      </c>
+      <c r="J118" s="69">
+        <v>30</v>
+      </c>
+      <c r="K118" s="66"/>
+      <c r="L118" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="M118" s="69">
+        <v>30</v>
+      </c>
+      <c r="N118" s="66"/>
+      <c r="O118" s="66"/>
+      <c r="P118" s="69">
+        <v>0</v>
+      </c>
+      <c r="Q118" s="69">
+        <v>17</v>
+      </c>
+      <c r="R118" s="66"/>
+      <c r="S118" s="66"/>
+      <c r="T118" s="66" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A119" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B119" s="66"/>
+      <c r="C119" s="66"/>
+      <c r="D119" s="67">
+        <v>43538</v>
+      </c>
+      <c r="E119" s="68" t="s">
+        <v>229</v>
+      </c>
+      <c r="F119" s="66" t="s">
+        <v>226</v>
+      </c>
+      <c r="G119" s="69">
+        <v>2</v>
+      </c>
+      <c r="H119" s="66"/>
+      <c r="I119" s="68" t="s">
+        <v>227</v>
+      </c>
+      <c r="J119" s="69">
+        <v>10</v>
+      </c>
+      <c r="K119" s="66"/>
+      <c r="L119" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="M119" s="69">
+        <v>30</v>
+      </c>
+      <c r="N119" s="66"/>
+      <c r="O119" s="66"/>
+      <c r="P119" s="69">
+        <v>0</v>
+      </c>
+      <c r="Q119" s="69">
+        <v>17</v>
+      </c>
+      <c r="R119" s="66"/>
+      <c r="S119" s="66"/>
+      <c r="T119" s="66" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A120" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B120" s="40"/>
+      <c r="C120" s="40"/>
+      <c r="D120" s="41">
+        <v>43573</v>
+      </c>
+      <c r="E120" s="70" t="s">
+        <v>230</v>
+      </c>
+      <c r="F120" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="G120" s="71">
+        <v>1</v>
+      </c>
+      <c r="H120" s="40"/>
+      <c r="I120" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="J120" s="71">
+        <v>30</v>
+      </c>
+      <c r="K120" s="71">
+        <v>15</v>
+      </c>
+      <c r="L120" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="M120" s="71">
+        <v>20</v>
+      </c>
+      <c r="N120" s="40"/>
+      <c r="O120" s="40"/>
+      <c r="P120" s="71">
+        <v>873</v>
+      </c>
+      <c r="Q120" s="71">
+        <v>17</v>
+      </c>
+      <c r="R120" s="40"/>
+      <c r="S120" s="40"/>
+      <c r="T120" s="40" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A121" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B121" s="40"/>
+      <c r="C121" s="40"/>
+      <c r="D121" s="41">
+        <v>43573</v>
+      </c>
+      <c r="E121" s="70" t="s">
+        <v>233</v>
+      </c>
+      <c r="F121" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="G121" s="71">
+        <v>2</v>
+      </c>
+      <c r="H121" s="40"/>
+      <c r="I121" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="J121" s="71">
+        <v>30</v>
+      </c>
+      <c r="K121" s="71">
+        <v>15</v>
+      </c>
+      <c r="L121" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="M121" s="71">
+        <v>40</v>
+      </c>
+      <c r="N121" s="40"/>
+      <c r="O121" s="40"/>
+      <c r="P121" s="71">
+        <v>873</v>
+      </c>
+      <c r="Q121" s="71">
+        <v>17</v>
+      </c>
+      <c r="R121" s="40"/>
+      <c r="S121" s="40"/>
+      <c r="T121" s="40" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A122" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B122" s="40"/>
+      <c r="C122" s="40"/>
+      <c r="D122" s="41">
+        <v>43573</v>
+      </c>
+      <c r="E122" s="70" t="s">
+        <v>234</v>
+      </c>
+      <c r="F122" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="G122" s="71">
+        <v>3</v>
+      </c>
+      <c r="H122" s="40"/>
+      <c r="I122" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="J122" s="71">
+        <v>30</v>
+      </c>
+      <c r="K122" s="71">
+        <v>15</v>
+      </c>
+      <c r="L122" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="M122" s="71">
+        <v>90</v>
+      </c>
+      <c r="N122" s="40"/>
+      <c r="O122" s="40"/>
+      <c r="P122" s="71">
+        <v>873</v>
+      </c>
+      <c r="Q122" s="71">
+        <v>17</v>
+      </c>
+      <c r="R122" s="40"/>
+      <c r="S122" s="40"/>
+      <c r="T122" s="40" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A123" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B123" s="40"/>
+      <c r="C123" s="40"/>
+      <c r="D123" s="41">
+        <v>43573</v>
+      </c>
+      <c r="E123" s="70" t="s">
+        <v>235</v>
+      </c>
+      <c r="F123" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="G123" s="71">
+        <v>4</v>
+      </c>
+      <c r="H123" s="40"/>
+      <c r="I123" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="J123" s="71">
+        <v>30</v>
+      </c>
+      <c r="K123" s="71">
+        <v>15</v>
+      </c>
+      <c r="L123" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="M123" s="71">
+        <v>60</v>
+      </c>
+      <c r="N123" s="40"/>
+      <c r="O123" s="40"/>
+      <c r="P123" s="71">
+        <v>873</v>
+      </c>
+      <c r="Q123" s="71">
+        <v>17</v>
+      </c>
+      <c r="R123" s="40"/>
+      <c r="S123" s="40"/>
+      <c r="T123" s="40" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A124" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B124" s="47"/>
+      <c r="C124" s="47"/>
+      <c r="D124" s="48">
+        <v>43580</v>
+      </c>
+      <c r="E124" s="72" t="s">
+        <v>238</v>
+      </c>
+      <c r="F124" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="G124" s="50">
+        <v>1</v>
+      </c>
+      <c r="H124" s="47"/>
+      <c r="I124" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="J124" s="50">
+        <v>5</v>
+      </c>
+      <c r="K124" s="50">
+        <v>15</v>
+      </c>
+      <c r="L124" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="M124" s="50">
+        <v>30</v>
+      </c>
+      <c r="N124" s="47"/>
+      <c r="O124" s="47"/>
+      <c r="P124" s="50">
+        <v>0</v>
+      </c>
+      <c r="Q124" s="50">
+        <v>17</v>
+      </c>
+      <c r="R124" s="47"/>
+      <c r="S124" s="47"/>
+      <c r="T124" s="47" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A125" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B125" s="47"/>
+      <c r="C125" s="47"/>
+      <c r="D125" s="48">
+        <v>43580</v>
+      </c>
+      <c r="E125" s="72" t="s">
+        <v>240</v>
+      </c>
+      <c r="F125" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="G125" s="50">
+        <v>2</v>
+      </c>
+      <c r="H125" s="47"/>
+      <c r="I125" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="J125" s="50">
+        <v>5</v>
+      </c>
+      <c r="K125" s="50">
+        <v>15</v>
+      </c>
+      <c r="L125" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="M125" s="50">
+        <v>30</v>
+      </c>
+      <c r="N125" s="47"/>
+      <c r="O125" s="47"/>
+      <c r="P125" s="50">
+        <v>873</v>
+      </c>
+      <c r="Q125" s="50">
+        <v>17</v>
+      </c>
+      <c r="R125" s="47"/>
+      <c r="S125" s="47"/>
+      <c r="T125" s="47" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A126" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B126" s="47"/>
+      <c r="C126" s="47"/>
+      <c r="D126" s="48">
+        <v>43581</v>
+      </c>
+      <c r="E126" s="72" t="s">
+        <v>243</v>
+      </c>
+      <c r="F126" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="G126" s="50">
+        <v>3</v>
+      </c>
+      <c r="H126" s="47"/>
+      <c r="I126" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="J126" s="50">
+        <v>5</v>
+      </c>
+      <c r="K126" s="50">
+        <v>15</v>
+      </c>
+      <c r="L126" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="M126" s="50">
+        <v>30</v>
+      </c>
+      <c r="N126" s="47"/>
+      <c r="O126" s="47"/>
+      <c r="P126" s="50">
+        <v>873</v>
+      </c>
+      <c r="Q126" s="50">
+        <v>17</v>
+      </c>
+      <c r="R126" s="47"/>
+      <c r="S126" s="47"/>
+      <c r="T126" s="47" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A127" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="B127" s="60"/>
+      <c r="C127" s="60"/>
+      <c r="D127" s="61">
+        <v>43581</v>
+      </c>
+      <c r="E127" s="62" t="s">
+        <v>245</v>
+      </c>
+      <c r="F127" s="60" t="s">
+        <v>246</v>
+      </c>
+      <c r="G127" s="63">
+        <v>1</v>
+      </c>
+      <c r="H127" s="60"/>
+      <c r="I127" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="J127" s="63">
+        <v>30</v>
+      </c>
+      <c r="K127" s="60"/>
+      <c r="L127" s="60"/>
+      <c r="M127" s="60"/>
+      <c r="N127" s="60"/>
+      <c r="O127" s="60"/>
+      <c r="P127" s="60"/>
+      <c r="Q127" s="63">
+        <v>17</v>
+      </c>
+      <c r="R127" s="60"/>
+      <c r="S127" s="60"/>
+      <c r="T127" s="60" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -7459,7 +8003,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>

</xml_diff>

<commit_message>
Script for resistance measurement with a voice that reads the resistance value
</commit_message>
<xml_diff>
--- a/ivtools/sampledata/CeRAM_Depositions.xlsx
+++ b/ivtools/sampledata/CeRAM_Depositions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="253">
   <si>
     <t>wafer_number</t>
   </si>
@@ -763,16 +763,28 @@
     <t>Dachs</t>
   </si>
   <si>
-    <t>contact test</t>
-  </si>
-  <si>
     <t>TE thickness variation, additional 60nm Pt added 2019-04-26</t>
+  </si>
+  <si>
+    <t>Dachs2</t>
+  </si>
+  <si>
+    <t>Dachs3</t>
+  </si>
+  <si>
+    <t>corner piece; contact test</t>
+  </si>
+  <si>
+    <t>corner piece; contact test, etched with option "reduce pump speed = yes"</t>
+  </si>
+  <si>
+    <t>corner piece; contact test, etched with option "reduce pump speed = no"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1478,48 +1490,48 @@
     <xf numFmtId="2" fontId="0" fillId="52" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1802,14 +1814,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T127"/>
+  <dimension ref="A1:T129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M123" sqref="M123"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M132" sqref="M132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -7754,7 +7766,7 @@
       <c r="R122" s="40"/>
       <c r="S122" s="40"/>
       <c r="T122" s="40" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.25">
@@ -7986,7 +7998,87 @@
       <c r="R127" s="60"/>
       <c r="S127" s="60"/>
       <c r="T127" s="60" t="s">
-        <v>247</v>
+        <v>250</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A128" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="B128" s="60"/>
+      <c r="C128" s="60"/>
+      <c r="D128" s="61">
+        <v>43608</v>
+      </c>
+      <c r="E128" s="62" t="s">
+        <v>248</v>
+      </c>
+      <c r="F128" s="60" t="s">
+        <v>246</v>
+      </c>
+      <c r="G128" s="63">
+        <v>2</v>
+      </c>
+      <c r="H128" s="60"/>
+      <c r="I128" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="J128" s="63">
+        <v>30</v>
+      </c>
+      <c r="K128" s="60"/>
+      <c r="L128" s="60"/>
+      <c r="M128" s="60"/>
+      <c r="N128" s="60"/>
+      <c r="O128" s="60"/>
+      <c r="P128" s="60"/>
+      <c r="Q128" s="63">
+        <v>17</v>
+      </c>
+      <c r="R128" s="60"/>
+      <c r="S128" s="60"/>
+      <c r="T128" s="60" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A129" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="B129" s="60"/>
+      <c r="C129" s="60"/>
+      <c r="D129" s="61">
+        <v>43609</v>
+      </c>
+      <c r="E129" s="62" t="s">
+        <v>249</v>
+      </c>
+      <c r="F129" s="60" t="s">
+        <v>246</v>
+      </c>
+      <c r="G129" s="63">
+        <v>3</v>
+      </c>
+      <c r="H129" s="60"/>
+      <c r="I129" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="J129" s="63">
+        <v>30</v>
+      </c>
+      <c r="K129" s="60"/>
+      <c r="L129" s="60"/>
+      <c r="M129" s="60"/>
+      <c r="N129" s="60"/>
+      <c r="O129" s="60"/>
+      <c r="P129" s="60"/>
+      <c r="Q129" s="63">
+        <v>17</v>
+      </c>
+      <c r="R129" s="60"/>
+      <c r="S129" s="60"/>
+      <c r="T129" s="60" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -8003,7 +8095,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>

</xml_diff>

<commit_message>
fix incorrect timestamp in chplotter, femto log amp added
</commit_message>
<xml_diff>
--- a/ivtools/sampledata/CeRAM_Depositions.xlsx
+++ b/ivtools/sampledata/CeRAM_Depositions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\emrl\Pool\Projekte\HGST-CERAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\t\py-ivtools\ivtools\sampledata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="263">
   <si>
     <t>wafer_number</t>
   </si>
@@ -779,12 +779,42 @@
   </si>
   <si>
     <t>corner piece; contact test, etched with option "reduce pump speed = no"</t>
+  </si>
+  <si>
+    <t>Ahorn3</t>
+  </si>
+  <si>
+    <t>NiO more gas flow</t>
+  </si>
+  <si>
+    <t>MFC1</t>
+  </si>
+  <si>
+    <t>MFC2</t>
+  </si>
+  <si>
+    <t>MFC1_gas</t>
+  </si>
+  <si>
+    <t>MFC2_gas</t>
+  </si>
+  <si>
+    <t>dep_pressure</t>
+  </si>
+  <si>
+    <t>dep_power</t>
+  </si>
+  <si>
+    <t>Ar</t>
+  </si>
+  <si>
+    <t>1%O2/99%Ar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1490,48 +1520,48 @@
     <xf numFmtId="2" fontId="0" fillId="52" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1814,14 +1844,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T129"/>
+  <dimension ref="A1:Z130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M132" sqref="M132"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V119" sqref="V119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -1839,46 +1869,46 @@
     <col min="16" max="16" width="22.7109375" customWidth="1"/>
     <col min="17" max="17" width="15.42578125" customWidth="1"/>
     <col min="18" max="18" width="13" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="103.5703125" customWidth="1"/>
+    <col min="19" max="25" width="15.7109375" customWidth="1"/>
+    <col min="26" max="26" width="103.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1894,11 +1924,11 @@
       <c r="P8" t="s">
         <v>91</v>
       </c>
-      <c r="T8" t="s">
+      <c r="Z8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>82</v>
       </c>
@@ -1957,10 +1987,28 @@
         <v>154</v>
       </c>
       <c r="T9" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="U9" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="V9" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="W9" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="X9" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y9" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="Z9" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1991,8 +2039,14 @@
       </c>
       <c r="S10" s="13"/>
       <c r="T10" s="13"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>83</v>
       </c>
@@ -2038,11 +2092,17 @@
         <v>94.5</v>
       </c>
       <c r="S11" s="2"/>
-      <c r="T11" s="2" t="s">
+      <c r="T11" s="2"/>
+      <c r="U11" s="2"/>
+      <c r="V11" s="2"/>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2"/>
+      <c r="Y11" s="2"/>
+      <c r="Z11" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>83</v>
       </c>
@@ -2088,11 +2148,17 @@
         <v>76.5</v>
       </c>
       <c r="S12" s="2"/>
-      <c r="T12" s="2" t="s">
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
+      <c r="V12" s="2"/>
+      <c r="W12" s="2"/>
+      <c r="X12" s="2"/>
+      <c r="Y12" s="2"/>
+      <c r="Z12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>83</v>
       </c>
@@ -2138,11 +2204,17 @@
         <v>58.5</v>
       </c>
       <c r="S13" s="2"/>
-      <c r="T13" s="2" t="s">
+      <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
+      <c r="V13" s="2"/>
+      <c r="W13" s="2"/>
+      <c r="X13" s="2"/>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>83</v>
       </c>
@@ -2188,11 +2260,17 @@
         <v>40.5</v>
       </c>
       <c r="S14" s="2"/>
-      <c r="T14" s="2" t="s">
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
+      <c r="W14" s="2"/>
+      <c r="X14" s="2"/>
+      <c r="Y14" s="2"/>
+      <c r="Z14" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>83</v>
       </c>
@@ -2244,11 +2322,17 @@
         <v>76.5</v>
       </c>
       <c r="S15" s="1"/>
-      <c r="T15" s="1" t="s">
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>83</v>
       </c>
@@ -2300,11 +2384,17 @@
         <v>76.5</v>
       </c>
       <c r="S16" s="1"/>
-      <c r="T16" s="1" t="s">
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>83</v>
       </c>
@@ -2356,11 +2446,17 @@
         <v>76.5</v>
       </c>
       <c r="S17" s="1"/>
-      <c r="T17" s="1" t="s">
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>83</v>
       </c>
@@ -2412,11 +2508,17 @@
         <v>76.5</v>
       </c>
       <c r="S18" s="1"/>
-      <c r="T18" s="1" t="s">
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>83</v>
       </c>
@@ -2468,11 +2570,17 @@
         <v>76.5</v>
       </c>
       <c r="S19" s="1"/>
-      <c r="T19" s="1" t="s">
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>83</v>
       </c>
@@ -2524,11 +2632,17 @@
         <v>76.5</v>
       </c>
       <c r="S20" s="1"/>
-      <c r="T20" s="1" t="s">
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>83</v>
       </c>
@@ -2580,11 +2694,17 @@
         <v>76.5</v>
       </c>
       <c r="S21" s="16"/>
-      <c r="T21" s="16" t="s">
+      <c r="T21" s="16"/>
+      <c r="U21" s="16"/>
+      <c r="V21" s="16"/>
+      <c r="W21" s="16"/>
+      <c r="X21" s="16"/>
+      <c r="Y21" s="16"/>
+      <c r="Z21" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>83</v>
       </c>
@@ -2636,11 +2756,17 @@
         <v>76.5</v>
       </c>
       <c r="S22" s="16"/>
-      <c r="T22" s="16" t="s">
+      <c r="T22" s="16"/>
+      <c r="U22" s="16"/>
+      <c r="V22" s="16"/>
+      <c r="W22" s="16"/>
+      <c r="X22" s="16"/>
+      <c r="Y22" s="16"/>
+      <c r="Z22" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>83</v>
       </c>
@@ -2692,11 +2818,17 @@
         <v>76.5</v>
       </c>
       <c r="S23" s="16"/>
-      <c r="T23" s="16" t="s">
+      <c r="T23" s="16"/>
+      <c r="U23" s="16"/>
+      <c r="V23" s="16"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>83</v>
       </c>
@@ -2748,11 +2880,17 @@
         <v>76.5</v>
       </c>
       <c r="S24" s="16"/>
-      <c r="T24" s="16" t="s">
+      <c r="T24" s="16"/>
+      <c r="U24" s="16"/>
+      <c r="V24" s="16"/>
+      <c r="W24" s="16"/>
+      <c r="X24" s="16"/>
+      <c r="Y24" s="16"/>
+      <c r="Z24" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>83</v>
       </c>
@@ -2804,11 +2942,17 @@
         <v>76.5</v>
       </c>
       <c r="S25" s="16"/>
-      <c r="T25" s="16" t="s">
+      <c r="T25" s="16"/>
+      <c r="U25" s="16"/>
+      <c r="V25" s="16"/>
+      <c r="W25" s="16"/>
+      <c r="X25" s="16"/>
+      <c r="Y25" s="16"/>
+      <c r="Z25" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>83</v>
       </c>
@@ -2860,11 +3004,17 @@
         <v>76.5</v>
       </c>
       <c r="S26" s="16"/>
-      <c r="T26" s="16" t="s">
+      <c r="T26" s="16"/>
+      <c r="U26" s="16"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="16"/>
+      <c r="X26" s="16"/>
+      <c r="Y26" s="16"/>
+      <c r="Z26" s="16" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>83</v>
       </c>
@@ -2910,11 +3060,17 @@
         <v>76.5</v>
       </c>
       <c r="S27" s="11"/>
-      <c r="T27" s="11" t="s">
+      <c r="T27" s="11"/>
+      <c r="U27" s="11"/>
+      <c r="V27" s="11"/>
+      <c r="W27" s="11"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="11"/>
+      <c r="Z27" s="11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>83</v>
       </c>
@@ -2966,11 +3122,17 @@
         <v>76.5</v>
       </c>
       <c r="S28" s="8"/>
-      <c r="T28" s="8" t="s">
+      <c r="T28" s="8"/>
+      <c r="U28" s="8"/>
+      <c r="V28" s="8"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="8"/>
+      <c r="Y28" s="8"/>
+      <c r="Z28" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>83</v>
       </c>
@@ -3014,11 +3176,17 @@
         <v>76.5</v>
       </c>
       <c r="S29" s="6"/>
-      <c r="T29" s="6" t="s">
+      <c r="T29" s="6"/>
+      <c r="U29" s="6"/>
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+      <c r="X29" s="6"/>
+      <c r="Y29" s="6"/>
+      <c r="Z29" s="6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>83</v>
       </c>
@@ -3064,11 +3232,17 @@
         <v>0</v>
       </c>
       <c r="S30" s="2"/>
-      <c r="T30" s="2" t="s">
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>83</v>
       </c>
@@ -3120,11 +3294,17 @@
         <v>76.5</v>
       </c>
       <c r="S31" s="14"/>
-      <c r="T31" s="14" t="s">
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="14"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="14"/>
+      <c r="Z31" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>83</v>
       </c>
@@ -3176,11 +3356,17 @@
         <v>76.5</v>
       </c>
       <c r="S32" s="14"/>
-      <c r="T32" s="14" t="s">
+      <c r="T32" s="14"/>
+      <c r="U32" s="14"/>
+      <c r="V32" s="14"/>
+      <c r="W32" s="14"/>
+      <c r="X32" s="14"/>
+      <c r="Y32" s="14"/>
+      <c r="Z32" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>83</v>
       </c>
@@ -3232,11 +3418,17 @@
         <v>76.5</v>
       </c>
       <c r="S33" s="14"/>
-      <c r="T33" s="14" t="s">
+      <c r="T33" s="14"/>
+      <c r="U33" s="14"/>
+      <c r="V33" s="14"/>
+      <c r="W33" s="14"/>
+      <c r="X33" s="14"/>
+      <c r="Y33" s="14"/>
+      <c r="Z33" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>83</v>
       </c>
@@ -3288,11 +3480,17 @@
         <v>76.5</v>
       </c>
       <c r="S34" s="14"/>
-      <c r="T34" s="14" t="s">
+      <c r="T34" s="14"/>
+      <c r="U34" s="14"/>
+      <c r="V34" s="14"/>
+      <c r="W34" s="14"/>
+      <c r="X34" s="14"/>
+      <c r="Y34" s="14"/>
+      <c r="Z34" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>83</v>
       </c>
@@ -3344,11 +3542,17 @@
         <v>76.5</v>
       </c>
       <c r="S35" s="14"/>
-      <c r="T35" s="14" t="s">
+      <c r="T35" s="14"/>
+      <c r="U35" s="14"/>
+      <c r="V35" s="14"/>
+      <c r="W35" s="14"/>
+      <c r="X35" s="14"/>
+      <c r="Y35" s="14"/>
+      <c r="Z35" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>83</v>
       </c>
@@ -3400,11 +3604,17 @@
         <v>76.5</v>
       </c>
       <c r="S36" s="14"/>
-      <c r="T36" s="14" t="s">
+      <c r="T36" s="14"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="14"/>
+      <c r="X36" s="14"/>
+      <c r="Y36" s="14"/>
+      <c r="Z36" s="14" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>83</v>
       </c>
@@ -3456,11 +3666,17 @@
         <v>76.5</v>
       </c>
       <c r="S37" s="18"/>
-      <c r="T37" s="18" t="s">
+      <c r="T37" s="18"/>
+      <c r="U37" s="18"/>
+      <c r="V37" s="18"/>
+      <c r="W37" s="18"/>
+      <c r="X37" s="18"/>
+      <c r="Y37" s="18"/>
+      <c r="Z37" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>83</v>
       </c>
@@ -3512,11 +3728,17 @@
         <v>76.5</v>
       </c>
       <c r="S38" s="18"/>
-      <c r="T38" s="18" t="s">
+      <c r="T38" s="18"/>
+      <c r="U38" s="18"/>
+      <c r="V38" s="18"/>
+      <c r="W38" s="18"/>
+      <c r="X38" s="18"/>
+      <c r="Y38" s="18"/>
+      <c r="Z38" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>83</v>
       </c>
@@ -3568,11 +3790,17 @@
         <v>76.5</v>
       </c>
       <c r="S39" s="18"/>
-      <c r="T39" s="18" t="s">
+      <c r="T39" s="18"/>
+      <c r="U39" s="18"/>
+      <c r="V39" s="18"/>
+      <c r="W39" s="18"/>
+      <c r="X39" s="18"/>
+      <c r="Y39" s="18"/>
+      <c r="Z39" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>83</v>
       </c>
@@ -3624,11 +3852,17 @@
         <v>76.5</v>
       </c>
       <c r="S40" s="18"/>
-      <c r="T40" s="18" t="s">
+      <c r="T40" s="18"/>
+      <c r="U40" s="18"/>
+      <c r="V40" s="18"/>
+      <c r="W40" s="18"/>
+      <c r="X40" s="18"/>
+      <c r="Y40" s="18"/>
+      <c r="Z40" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>83</v>
       </c>
@@ -3680,11 +3914,17 @@
         <v>76.5</v>
       </c>
       <c r="S41" s="18"/>
-      <c r="T41" s="18" t="s">
+      <c r="T41" s="18"/>
+      <c r="U41" s="18"/>
+      <c r="V41" s="18"/>
+      <c r="W41" s="18"/>
+      <c r="X41" s="18"/>
+      <c r="Y41" s="18"/>
+      <c r="Z41" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>83</v>
       </c>
@@ -3736,11 +3976,17 @@
         <v>76.5</v>
       </c>
       <c r="S42" s="18"/>
-      <c r="T42" s="18" t="s">
+      <c r="T42" s="18"/>
+      <c r="U42" s="18"/>
+      <c r="V42" s="18"/>
+      <c r="W42" s="18"/>
+      <c r="X42" s="18"/>
+      <c r="Y42" s="18"/>
+      <c r="Z42" s="18" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>100</v>
       </c>
@@ -3780,11 +4026,17 @@
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
       <c r="S43" s="1"/>
-      <c r="T43" s="1" t="s">
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>100</v>
       </c>
@@ -3824,11 +4076,17 @@
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
       <c r="S44" s="1"/>
-      <c r="T44" s="1" t="s">
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>100</v>
       </c>
@@ -3868,11 +4126,17 @@
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
       <c r="S45" s="1"/>
-      <c r="T45" s="1" t="s">
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>100</v>
       </c>
@@ -3912,11 +4176,17 @@
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
       <c r="S46" s="1"/>
-      <c r="T46" s="1" t="s">
+      <c r="T46" s="1"/>
+      <c r="U46" s="1"/>
+      <c r="V46" s="1"/>
+      <c r="W46" s="1"/>
+      <c r="X46" s="1"/>
+      <c r="Y46" s="1"/>
+      <c r="Z46" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>100</v>
       </c>
@@ -3956,11 +4226,17 @@
       <c r="Q47" s="1"/>
       <c r="R47" s="1"/>
       <c r="S47" s="1"/>
-      <c r="T47" s="1" t="s">
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>100</v>
       </c>
@@ -4000,11 +4276,17 @@
       <c r="Q48" s="1"/>
       <c r="R48" s="1"/>
       <c r="S48" s="1"/>
-      <c r="T48" s="1" t="s">
+      <c r="T48" s="1"/>
+      <c r="U48" s="1"/>
+      <c r="V48" s="1"/>
+      <c r="W48" s="1"/>
+      <c r="X48" s="1"/>
+      <c r="Y48" s="1"/>
+      <c r="Z48" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="20" t="s">
         <v>83</v>
       </c>
@@ -4056,11 +4338,17 @@
       <c r="S49" s="20">
         <v>500</v>
       </c>
-      <c r="T49" s="20" t="s">
+      <c r="T49" s="20"/>
+      <c r="U49" s="20"/>
+      <c r="V49" s="20"/>
+      <c r="W49" s="20"/>
+      <c r="X49" s="20"/>
+      <c r="Y49" s="20"/>
+      <c r="Z49" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="20" t="s">
         <v>83</v>
       </c>
@@ -4112,11 +4400,17 @@
       <c r="S50" s="20">
         <v>500</v>
       </c>
-      <c r="T50" s="20" t="s">
+      <c r="T50" s="20"/>
+      <c r="U50" s="20"/>
+      <c r="V50" s="20"/>
+      <c r="W50" s="20"/>
+      <c r="X50" s="20"/>
+      <c r="Y50" s="20"/>
+      <c r="Z50" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>83</v>
       </c>
@@ -4168,11 +4462,17 @@
       <c r="S51" s="20">
         <v>500</v>
       </c>
-      <c r="T51" s="20" t="s">
+      <c r="T51" s="20"/>
+      <c r="U51" s="20"/>
+      <c r="V51" s="20"/>
+      <c r="W51" s="20"/>
+      <c r="X51" s="20"/>
+      <c r="Y51" s="20"/>
+      <c r="Z51" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>83</v>
       </c>
@@ -4224,11 +4524,17 @@
       <c r="S52" s="20">
         <v>500</v>
       </c>
-      <c r="T52" s="20" t="s">
+      <c r="T52" s="20"/>
+      <c r="U52" s="20"/>
+      <c r="V52" s="20"/>
+      <c r="W52" s="20"/>
+      <c r="X52" s="20"/>
+      <c r="Y52" s="20"/>
+      <c r="Z52" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="20" t="s">
         <v>83</v>
       </c>
@@ -4280,11 +4586,17 @@
       <c r="S53" s="20">
         <v>500</v>
       </c>
-      <c r="T53" s="20" t="s">
+      <c r="T53" s="20"/>
+      <c r="U53" s="20"/>
+      <c r="V53" s="20"/>
+      <c r="W53" s="20"/>
+      <c r="X53" s="20"/>
+      <c r="Y53" s="20"/>
+      <c r="Z53" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="20" t="s">
         <v>83</v>
       </c>
@@ -4336,11 +4648,17 @@
       <c r="S54" s="20">
         <v>500</v>
       </c>
-      <c r="T54" s="20" t="s">
+      <c r="T54" s="20"/>
+      <c r="U54" s="20"/>
+      <c r="V54" s="20"/>
+      <c r="W54" s="20"/>
+      <c r="X54" s="20"/>
+      <c r="Y54" s="20"/>
+      <c r="Z54" s="20" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="22" t="s">
         <v>83</v>
       </c>
@@ -4386,11 +4704,17 @@
         <v>76.5</v>
       </c>
       <c r="S55" s="22"/>
-      <c r="T55" s="22" t="s">
+      <c r="T55" s="22"/>
+      <c r="U55" s="22"/>
+      <c r="V55" s="22"/>
+      <c r="W55" s="22"/>
+      <c r="X55" s="22"/>
+      <c r="Y55" s="22"/>
+      <c r="Z55" s="22" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
         <v>83</v>
       </c>
@@ -4440,11 +4764,17 @@
         <v>76.5</v>
       </c>
       <c r="S56" s="22"/>
-      <c r="T56" s="22" t="s">
+      <c r="T56" s="22"/>
+      <c r="U56" s="22"/>
+      <c r="V56" s="22"/>
+      <c r="W56" s="22"/>
+      <c r="X56" s="22"/>
+      <c r="Y56" s="22"/>
+      <c r="Z56" s="22" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>100</v>
       </c>
@@ -4484,11 +4814,17 @@
       <c r="Q57" s="1"/>
       <c r="R57" s="1"/>
       <c r="S57" s="1"/>
-      <c r="T57" s="1" t="s">
+      <c r="T57" s="1"/>
+      <c r="U57" s="1"/>
+      <c r="V57" s="1"/>
+      <c r="W57" s="1"/>
+      <c r="X57" s="1"/>
+      <c r="Y57" s="1"/>
+      <c r="Z57" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>100</v>
       </c>
@@ -4528,11 +4864,17 @@
       <c r="Q58" s="1"/>
       <c r="R58" s="1"/>
       <c r="S58" s="1"/>
-      <c r="T58" s="1" t="s">
+      <c r="T58" s="1"/>
+      <c r="U58" s="1"/>
+      <c r="V58" s="1"/>
+      <c r="W58" s="1"/>
+      <c r="X58" s="1"/>
+      <c r="Y58" s="1"/>
+      <c r="Z58" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>100</v>
       </c>
@@ -4572,11 +4914,17 @@
       <c r="Q59" s="1"/>
       <c r="R59" s="1"/>
       <c r="S59" s="1"/>
-      <c r="T59" s="1" t="s">
+      <c r="T59" s="1"/>
+      <c r="U59" s="1"/>
+      <c r="V59" s="1"/>
+      <c r="W59" s="1"/>
+      <c r="X59" s="1"/>
+      <c r="Y59" s="1"/>
+      <c r="Z59" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>100</v>
       </c>
@@ -4616,11 +4964,17 @@
       <c r="Q60" s="1"/>
       <c r="R60" s="1"/>
       <c r="S60" s="1"/>
-      <c r="T60" s="1" t="s">
+      <c r="T60" s="1"/>
+      <c r="U60" s="1"/>
+      <c r="V60" s="1"/>
+      <c r="W60" s="1"/>
+      <c r="X60" s="1"/>
+      <c r="Y60" s="1"/>
+      <c r="Z60" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>100</v>
       </c>
@@ -4660,11 +5014,17 @@
       <c r="Q61" s="1"/>
       <c r="R61" s="1"/>
       <c r="S61" s="1"/>
-      <c r="T61" s="1" t="s">
+      <c r="T61" s="1"/>
+      <c r="U61" s="1"/>
+      <c r="V61" s="1"/>
+      <c r="W61" s="1"/>
+      <c r="X61" s="1"/>
+      <c r="Y61" s="1"/>
+      <c r="Z61" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>100</v>
       </c>
@@ -4704,11 +5064,17 @@
       <c r="Q62" s="1"/>
       <c r="R62" s="1"/>
       <c r="S62" s="1"/>
-      <c r="T62" s="1" t="s">
+      <c r="T62" s="1"/>
+      <c r="U62" s="1"/>
+      <c r="V62" s="1"/>
+      <c r="W62" s="1"/>
+      <c r="X62" s="1"/>
+      <c r="Y62" s="1"/>
+      <c r="Z62" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>83</v>
       </c>
@@ -4742,11 +5108,17 @@
       <c r="Q63" s="1"/>
       <c r="R63" s="1"/>
       <c r="S63" s="1"/>
-      <c r="T63" s="1" t="s">
+      <c r="T63" s="1"/>
+      <c r="U63" s="1"/>
+      <c r="V63" s="1"/>
+      <c r="W63" s="1"/>
+      <c r="X63" s="1"/>
+      <c r="Y63" s="1"/>
+      <c r="Z63" s="1" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="20" t="s">
         <v>83</v>
       </c>
@@ -4796,11 +5168,17 @@
       <c r="S64" s="20">
         <v>500</v>
       </c>
-      <c r="T64" s="20" t="s">
+      <c r="T64" s="20"/>
+      <c r="U64" s="20"/>
+      <c r="V64" s="20"/>
+      <c r="W64" s="20"/>
+      <c r="X64" s="20"/>
+      <c r="Y64" s="20"/>
+      <c r="Z64" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="20" t="s">
         <v>83</v>
       </c>
@@ -4850,11 +5228,17 @@
       <c r="S65" s="20">
         <v>500</v>
       </c>
-      <c r="T65" s="20" t="s">
+      <c r="T65" s="20"/>
+      <c r="U65" s="20"/>
+      <c r="V65" s="20"/>
+      <c r="W65" s="20"/>
+      <c r="X65" s="20"/>
+      <c r="Y65" s="20"/>
+      <c r="Z65" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="20" t="s">
         <v>83</v>
       </c>
@@ -4904,11 +5288,17 @@
       <c r="S66" s="20">
         <v>500</v>
       </c>
-      <c r="T66" s="20" t="s">
+      <c r="T66" s="20"/>
+      <c r="U66" s="20"/>
+      <c r="V66" s="20"/>
+      <c r="W66" s="20"/>
+      <c r="X66" s="20"/>
+      <c r="Y66" s="20"/>
+      <c r="Z66" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="20" t="s">
         <v>83</v>
       </c>
@@ -4958,11 +5348,17 @@
       <c r="S67" s="20">
         <v>500</v>
       </c>
-      <c r="T67" s="20" t="s">
+      <c r="T67" s="20"/>
+      <c r="U67" s="20"/>
+      <c r="V67" s="20"/>
+      <c r="W67" s="20"/>
+      <c r="X67" s="20"/>
+      <c r="Y67" s="20"/>
+      <c r="Z67" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="20" t="s">
         <v>83</v>
       </c>
@@ -5012,11 +5408,17 @@
       <c r="S68" s="20">
         <v>500</v>
       </c>
-      <c r="T68" s="20" t="s">
+      <c r="T68" s="20"/>
+      <c r="U68" s="20"/>
+      <c r="V68" s="20"/>
+      <c r="W68" s="20"/>
+      <c r="X68" s="20"/>
+      <c r="Y68" s="20"/>
+      <c r="Z68" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="20" t="s">
         <v>83</v>
       </c>
@@ -5066,11 +5468,17 @@
       <c r="S69" s="20">
         <v>500</v>
       </c>
-      <c r="T69" s="20" t="s">
+      <c r="T69" s="20"/>
+      <c r="U69" s="20"/>
+      <c r="V69" s="20"/>
+      <c r="W69" s="20"/>
+      <c r="X69" s="20"/>
+      <c r="Y69" s="20"/>
+      <c r="Z69" s="20" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="24" t="s">
         <v>124</v>
       </c>
@@ -5106,11 +5514,17 @@
       <c r="Q70" s="24"/>
       <c r="R70" s="24"/>
       <c r="S70" s="24"/>
-      <c r="T70" s="24" t="s">
+      <c r="T70" s="24"/>
+      <c r="U70" s="24"/>
+      <c r="V70" s="24"/>
+      <c r="W70" s="24"/>
+      <c r="X70" s="24"/>
+      <c r="Y70" s="24"/>
+      <c r="Z70" s="24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
         <v>124</v>
       </c>
@@ -5152,11 +5566,17 @@
       <c r="Q71" s="24"/>
       <c r="R71" s="24"/>
       <c r="S71" s="24"/>
-      <c r="T71" s="24" t="s">
+      <c r="T71" s="24"/>
+      <c r="U71" s="24"/>
+      <c r="V71" s="24"/>
+      <c r="W71" s="24"/>
+      <c r="X71" s="24"/>
+      <c r="Y71" s="24"/>
+      <c r="Z71" s="24" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="24" t="s">
         <v>124</v>
       </c>
@@ -5198,11 +5618,17 @@
       <c r="Q72" s="24"/>
       <c r="R72" s="24"/>
       <c r="S72" s="24"/>
-      <c r="T72" s="24" t="s">
+      <c r="T72" s="24"/>
+      <c r="U72" s="24"/>
+      <c r="V72" s="24"/>
+      <c r="W72" s="24"/>
+      <c r="X72" s="24"/>
+      <c r="Y72" s="24"/>
+      <c r="Z72" s="24" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="24" t="s">
         <v>124</v>
       </c>
@@ -5244,11 +5670,17 @@
       <c r="Q73" s="24"/>
       <c r="R73" s="24"/>
       <c r="S73" s="24"/>
-      <c r="T73" s="24" t="s">
+      <c r="T73" s="24"/>
+      <c r="U73" s="24"/>
+      <c r="V73" s="24"/>
+      <c r="W73" s="24"/>
+      <c r="X73" s="24"/>
+      <c r="Y73" s="24"/>
+      <c r="Z73" s="24" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
         <v>83</v>
       </c>
@@ -5280,11 +5712,17 @@
       <c r="Q74" s="24"/>
       <c r="R74" s="24"/>
       <c r="S74" s="24"/>
-      <c r="T74" s="24" t="s">
+      <c r="T74" s="24"/>
+      <c r="U74" s="24"/>
+      <c r="V74" s="24"/>
+      <c r="W74" s="24"/>
+      <c r="X74" s="24"/>
+      <c r="Y74" s="24"/>
+      <c r="Z74" s="24" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="26" t="s">
         <v>83</v>
       </c>
@@ -5328,11 +5766,17 @@
       <c r="S75" s="26">
         <v>750</v>
       </c>
-      <c r="T75" s="26" t="s">
+      <c r="T75" s="26"/>
+      <c r="U75" s="26"/>
+      <c r="V75" s="26"/>
+      <c r="W75" s="26"/>
+      <c r="X75" s="26"/>
+      <c r="Y75" s="26"/>
+      <c r="Z75" s="26" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="26" t="s">
         <v>83</v>
       </c>
@@ -5376,11 +5820,17 @@
       <c r="S76" s="26">
         <v>750</v>
       </c>
-      <c r="T76" s="26" t="s">
+      <c r="T76" s="26"/>
+      <c r="U76" s="26"/>
+      <c r="V76" s="26"/>
+      <c r="W76" s="26"/>
+      <c r="X76" s="26"/>
+      <c r="Y76" s="26"/>
+      <c r="Z76" s="26" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="26" t="s">
         <v>139</v>
       </c>
@@ -5418,11 +5868,17 @@
       <c r="S77" s="26">
         <v>750</v>
       </c>
-      <c r="T77" s="26" t="s">
+      <c r="T77" s="26"/>
+      <c r="U77" s="26"/>
+      <c r="V77" s="26"/>
+      <c r="W77" s="26"/>
+      <c r="X77" s="26"/>
+      <c r="Y77" s="26"/>
+      <c r="Z77" s="26" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="26" t="s">
         <v>139</v>
       </c>
@@ -5460,11 +5916,17 @@
       <c r="S78" s="26">
         <v>750</v>
       </c>
-      <c r="T78" s="26" t="s">
+      <c r="T78" s="26"/>
+      <c r="U78" s="26"/>
+      <c r="V78" s="26"/>
+      <c r="W78" s="26"/>
+      <c r="X78" s="26"/>
+      <c r="Y78" s="26"/>
+      <c r="Z78" s="26" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="s">
         <v>83</v>
       </c>
@@ -5514,11 +5976,17 @@
         <v>76.5</v>
       </c>
       <c r="S79" s="30"/>
-      <c r="T79" s="30" t="s">
+      <c r="T79" s="30"/>
+      <c r="U79" s="30"/>
+      <c r="V79" s="30"/>
+      <c r="W79" s="30"/>
+      <c r="X79" s="30"/>
+      <c r="Y79" s="30"/>
+      <c r="Z79" s="30" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="32" t="s">
         <v>83</v>
       </c>
@@ -5564,11 +6032,17 @@
       <c r="S80" s="32">
         <v>500</v>
       </c>
-      <c r="T80" s="32" t="s">
+      <c r="T80" s="32"/>
+      <c r="U80" s="32"/>
+      <c r="V80" s="32"/>
+      <c r="W80" s="32"/>
+      <c r="X80" s="32"/>
+      <c r="Y80" s="32"/>
+      <c r="Z80" s="32" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="34" t="s">
         <v>83</v>
       </c>
@@ -5621,8 +6095,14 @@
       </c>
       <c r="S81" s="34"/>
       <c r="T81" s="34"/>
-    </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U81" s="34"/>
+      <c r="V81" s="34"/>
+      <c r="W81" s="34"/>
+      <c r="X81" s="34"/>
+      <c r="Y81" s="34"/>
+      <c r="Z81" s="34"/>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="34" t="s">
         <v>83</v>
       </c>
@@ -5675,8 +6155,14 @@
       </c>
       <c r="S82" s="34"/>
       <c r="T82" s="34"/>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U82" s="34"/>
+      <c r="V82" s="34"/>
+      <c r="W82" s="34"/>
+      <c r="X82" s="34"/>
+      <c r="Y82" s="34"/>
+      <c r="Z82" s="34"/>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="34" t="s">
         <v>83</v>
       </c>
@@ -5729,8 +6215,14 @@
       </c>
       <c r="S83" s="34"/>
       <c r="T83" s="34"/>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U83" s="34"/>
+      <c r="V83" s="34"/>
+      <c r="W83" s="34"/>
+      <c r="X83" s="34"/>
+      <c r="Y83" s="34"/>
+      <c r="Z83" s="34"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="37" t="s">
         <v>83</v>
       </c>
@@ -5782,11 +6274,17 @@
         <v>76.5</v>
       </c>
       <c r="S84" s="37"/>
-      <c r="T84" s="37" t="s">
+      <c r="T84" s="37"/>
+      <c r="U84" s="37"/>
+      <c r="V84" s="37"/>
+      <c r="W84" s="37"/>
+      <c r="X84" s="37"/>
+      <c r="Y84" s="37"/>
+      <c r="Z84" s="37" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="37" t="s">
         <v>83</v>
       </c>
@@ -5838,11 +6336,17 @@
         <v>76.5</v>
       </c>
       <c r="S85" s="37"/>
-      <c r="T85" s="37" t="s">
+      <c r="T85" s="37"/>
+      <c r="U85" s="37"/>
+      <c r="V85" s="37"/>
+      <c r="W85" s="37"/>
+      <c r="X85" s="37"/>
+      <c r="Y85" s="37"/>
+      <c r="Z85" s="37" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="37" t="s">
         <v>83</v>
       </c>
@@ -5894,11 +6398,17 @@
         <v>76.5</v>
       </c>
       <c r="S86" s="37"/>
-      <c r="T86" s="37" t="s">
+      <c r="T86" s="37"/>
+      <c r="U86" s="37"/>
+      <c r="V86" s="37"/>
+      <c r="W86" s="37"/>
+      <c r="X86" s="37"/>
+      <c r="Y86" s="37"/>
+      <c r="Z86" s="37" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="37" t="s">
         <v>83</v>
       </c>
@@ -5950,11 +6460,17 @@
         <v>76.5</v>
       </c>
       <c r="S87" s="37"/>
-      <c r="T87" s="37" t="s">
+      <c r="T87" s="37"/>
+      <c r="U87" s="37"/>
+      <c r="V87" s="37"/>
+      <c r="W87" s="37"/>
+      <c r="X87" s="37"/>
+      <c r="Y87" s="37"/>
+      <c r="Z87" s="37" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="37" t="s">
         <v>83</v>
       </c>
@@ -6006,11 +6522,17 @@
         <v>76.5</v>
       </c>
       <c r="S88" s="37"/>
-      <c r="T88" s="37" t="s">
+      <c r="T88" s="37"/>
+      <c r="U88" s="37"/>
+      <c r="V88" s="37"/>
+      <c r="W88" s="37"/>
+      <c r="X88" s="37"/>
+      <c r="Y88" s="37"/>
+      <c r="Z88" s="37" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="37" t="s">
         <v>83</v>
       </c>
@@ -6062,11 +6584,17 @@
         <v>76.5</v>
       </c>
       <c r="S89" s="37"/>
-      <c r="T89" s="37" t="s">
+      <c r="T89" s="37"/>
+      <c r="U89" s="37"/>
+      <c r="V89" s="37"/>
+      <c r="W89" s="37"/>
+      <c r="X89" s="37"/>
+      <c r="Y89" s="37"/>
+      <c r="Z89" s="37" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="40" t="s">
         <v>83</v>
       </c>
@@ -6118,11 +6646,17 @@
         <v>76.5</v>
       </c>
       <c r="S90" s="40"/>
-      <c r="T90" s="40" t="s">
+      <c r="T90" s="40"/>
+      <c r="U90" s="40"/>
+      <c r="V90" s="40"/>
+      <c r="W90" s="40"/>
+      <c r="X90" s="40"/>
+      <c r="Y90" s="40"/>
+      <c r="Z90" s="40" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="45" t="s">
         <v>83</v>
       </c>
@@ -6170,11 +6704,17 @@
         <v>76.5</v>
       </c>
       <c r="S91" s="49"/>
-      <c r="T91" s="45" t="s">
+      <c r="T91" s="49"/>
+      <c r="U91" s="49"/>
+      <c r="V91" s="49"/>
+      <c r="W91" s="49"/>
+      <c r="X91" s="49"/>
+      <c r="Y91" s="49"/>
+      <c r="Z91" s="45" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="45" t="s">
         <v>83</v>
       </c>
@@ -6222,11 +6762,17 @@
         <v>76.5</v>
       </c>
       <c r="S92" s="49"/>
-      <c r="T92" s="45" t="s">
+      <c r="T92" s="49"/>
+      <c r="U92" s="49"/>
+      <c r="V92" s="49"/>
+      <c r="W92" s="49"/>
+      <c r="X92" s="49"/>
+      <c r="Y92" s="49"/>
+      <c r="Z92" s="45" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="47" t="s">
         <v>83</v>
       </c>
@@ -6268,11 +6814,17 @@
         <v>0</v>
       </c>
       <c r="S93" s="50"/>
-      <c r="T93" s="47" t="s">
+      <c r="T93" s="50"/>
+      <c r="U93" s="50"/>
+      <c r="V93" s="50"/>
+      <c r="W93" s="50"/>
+      <c r="X93" s="50"/>
+      <c r="Y93" s="50"/>
+      <c r="Z93" s="47" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="47" t="s">
         <v>83</v>
       </c>
@@ -6314,11 +6866,17 @@
         <v>0</v>
       </c>
       <c r="S94" s="50"/>
-      <c r="T94" s="47" t="s">
+      <c r="T94" s="50"/>
+      <c r="U94" s="50"/>
+      <c r="V94" s="50"/>
+      <c r="W94" s="50"/>
+      <c r="X94" s="50"/>
+      <c r="Y94" s="50"/>
+      <c r="Z94" s="47" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="43" t="s">
         <v>83</v>
       </c>
@@ -6368,11 +6926,17 @@
         <v>76.5</v>
       </c>
       <c r="S95" s="43"/>
-      <c r="T95" s="43" t="s">
+      <c r="T95" s="43"/>
+      <c r="U95" s="43"/>
+      <c r="V95" s="43"/>
+      <c r="W95" s="43"/>
+      <c r="X95" s="43"/>
+      <c r="Y95" s="43"/>
+      <c r="Z95" s="43" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="43" t="s">
         <v>83</v>
       </c>
@@ -6422,11 +6986,17 @@
         <v>76.5</v>
       </c>
       <c r="S96" s="43"/>
-      <c r="T96" s="43" t="s">
+      <c r="T96" s="43"/>
+      <c r="U96" s="43"/>
+      <c r="V96" s="43"/>
+      <c r="W96" s="43"/>
+      <c r="X96" s="43"/>
+      <c r="Y96" s="43"/>
+      <c r="Z96" s="43" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="43" t="s">
         <v>83</v>
       </c>
@@ -6476,11 +7046,17 @@
         <v>76.5</v>
       </c>
       <c r="S97" s="43"/>
-      <c r="T97" s="43" t="s">
+      <c r="T97" s="43"/>
+      <c r="U97" s="43"/>
+      <c r="V97" s="43"/>
+      <c r="W97" s="43"/>
+      <c r="X97" s="43"/>
+      <c r="Y97" s="43"/>
+      <c r="Z97" s="43" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="43" t="s">
         <v>83</v>
       </c>
@@ -6530,11 +7106,17 @@
         <v>76.5</v>
       </c>
       <c r="S98" s="51"/>
-      <c r="T98" s="43" t="s">
+      <c r="T98" s="51"/>
+      <c r="U98" s="51"/>
+      <c r="V98" s="51"/>
+      <c r="W98" s="51"/>
+      <c r="X98" s="51"/>
+      <c r="Y98" s="51"/>
+      <c r="Z98" s="43" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="99" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A99" s="52" t="s">
         <v>83</v>
       </c>
@@ -6583,11 +7165,17 @@
         <v>76.5</v>
       </c>
       <c r="S99" s="55"/>
-      <c r="T99" s="54" t="s">
+      <c r="T99" s="55"/>
+      <c r="U99" s="55"/>
+      <c r="V99" s="55"/>
+      <c r="W99" s="55"/>
+      <c r="X99" s="55"/>
+      <c r="Y99" s="55"/>
+      <c r="Z99" s="54" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="100" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:26" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="52" t="s">
         <v>83</v>
       </c>
@@ -6636,11 +7224,17 @@
         <v>76.5</v>
       </c>
       <c r="S100" s="55"/>
-      <c r="T100" s="54" t="s">
+      <c r="T100" s="55"/>
+      <c r="U100" s="55"/>
+      <c r="V100" s="55"/>
+      <c r="W100" s="55"/>
+      <c r="X100" s="55"/>
+      <c r="Y100" s="55"/>
+      <c r="Z100" s="54" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="101" spans="1:20" s="52" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:26" s="52" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="52" t="s">
         <v>83</v>
       </c>
@@ -6689,11 +7283,17 @@
         <v>76.5</v>
       </c>
       <c r="S101" s="55"/>
-      <c r="T101" s="54" t="s">
+      <c r="T101" s="55"/>
+      <c r="U101" s="55"/>
+      <c r="V101" s="55"/>
+      <c r="W101" s="55"/>
+      <c r="X101" s="55"/>
+      <c r="Y101" s="55"/>
+      <c r="Z101" s="54" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A102" s="56" t="s">
         <v>83</v>
       </c>
@@ -6743,11 +7343,17 @@
         <v>76.5</v>
       </c>
       <c r="S102" s="59"/>
-      <c r="T102" s="58" t="s">
+      <c r="T102" s="59"/>
+      <c r="U102" s="59"/>
+      <c r="V102" s="59"/>
+      <c r="W102" s="59"/>
+      <c r="X102" s="59"/>
+      <c r="Y102" s="59"/>
+      <c r="Z102" s="58" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A103" s="56" t="s">
         <v>83</v>
       </c>
@@ -6797,11 +7403,17 @@
         <v>76.5</v>
       </c>
       <c r="S103" s="59"/>
-      <c r="T103" s="58" t="s">
+      <c r="T103" s="59"/>
+      <c r="U103" s="59"/>
+      <c r="V103" s="59"/>
+      <c r="W103" s="59"/>
+      <c r="X103" s="59"/>
+      <c r="Y103" s="59"/>
+      <c r="Z103" s="58" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A104" s="56" t="s">
         <v>83</v>
       </c>
@@ -6851,11 +7463,17 @@
         <v>76.5</v>
       </c>
       <c r="S104" s="59"/>
-      <c r="T104" s="58" t="s">
+      <c r="T104" s="59"/>
+      <c r="U104" s="59"/>
+      <c r="V104" s="59"/>
+      <c r="W104" s="59"/>
+      <c r="X104" s="59"/>
+      <c r="Y104" s="59"/>
+      <c r="Z104" s="58" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A105" s="56" t="s">
         <v>83</v>
       </c>
@@ -6905,11 +7523,17 @@
         <v>76.5</v>
       </c>
       <c r="S105" s="59"/>
-      <c r="T105" s="58" t="s">
+      <c r="T105" s="59"/>
+      <c r="U105" s="59"/>
+      <c r="V105" s="59"/>
+      <c r="W105" s="59"/>
+      <c r="X105" s="59"/>
+      <c r="Y105" s="59"/>
+      <c r="Z105" s="58" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A106" s="56" t="s">
         <v>83</v>
       </c>
@@ -6959,11 +7583,17 @@
         <v>76.5</v>
       </c>
       <c r="S106" s="59"/>
-      <c r="T106" s="58" t="s">
+      <c r="T106" s="59"/>
+      <c r="U106" s="59"/>
+      <c r="V106" s="59"/>
+      <c r="W106" s="59"/>
+      <c r="X106" s="59"/>
+      <c r="Y106" s="59"/>
+      <c r="Z106" s="58" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A107" s="56" t="s">
         <v>83</v>
       </c>
@@ -7013,11 +7643,17 @@
         <v>76.5</v>
       </c>
       <c r="S107" s="59"/>
-      <c r="T107" s="58" t="s">
+      <c r="T107" s="59"/>
+      <c r="U107" s="59"/>
+      <c r="V107" s="59"/>
+      <c r="W107" s="59"/>
+      <c r="X107" s="59"/>
+      <c r="Y107" s="59"/>
+      <c r="Z107" s="58" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A108" s="56" t="s">
         <v>83</v>
       </c>
@@ -7067,11 +7703,17 @@
         <v>76.5</v>
       </c>
       <c r="S108" s="59"/>
-      <c r="T108" s="58" t="s">
+      <c r="T108" s="59"/>
+      <c r="U108" s="59"/>
+      <c r="V108" s="59"/>
+      <c r="W108" s="59"/>
+      <c r="X108" s="59"/>
+      <c r="Y108" s="59"/>
+      <c r="Z108" s="58" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A109" s="56" t="s">
         <v>83</v>
       </c>
@@ -7121,11 +7763,17 @@
         <v>76.5</v>
       </c>
       <c r="S109" s="59"/>
-      <c r="T109" s="58" t="s">
+      <c r="T109" s="59"/>
+      <c r="U109" s="59"/>
+      <c r="V109" s="59"/>
+      <c r="W109" s="59"/>
+      <c r="X109" s="59"/>
+      <c r="Y109" s="59"/>
+      <c r="Z109" s="58" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A110" s="56" t="s">
         <v>83</v>
       </c>
@@ -7175,11 +7823,17 @@
         <v>76.5</v>
       </c>
       <c r="S110" s="59"/>
-      <c r="T110" s="58" t="s">
+      <c r="T110" s="59"/>
+      <c r="U110" s="59"/>
+      <c r="V110" s="59"/>
+      <c r="W110" s="59"/>
+      <c r="X110" s="59"/>
+      <c r="Y110" s="59"/>
+      <c r="Z110" s="58" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A111" s="56" t="s">
         <v>83</v>
       </c>
@@ -7229,11 +7883,17 @@
         <v>76.5</v>
       </c>
       <c r="S111" s="59"/>
-      <c r="T111" s="58" t="s">
+      <c r="T111" s="59"/>
+      <c r="U111" s="59"/>
+      <c r="V111" s="59"/>
+      <c r="W111" s="59"/>
+      <c r="X111" s="59"/>
+      <c r="Y111" s="59"/>
+      <c r="Z111" s="58" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A112" s="56" t="s">
         <v>83</v>
       </c>
@@ -7283,11 +7943,17 @@
         <v>76.5</v>
       </c>
       <c r="S112" s="59"/>
-      <c r="T112" s="58" t="s">
+      <c r="T112" s="59"/>
+      <c r="U112" s="59"/>
+      <c r="V112" s="59"/>
+      <c r="W112" s="59"/>
+      <c r="X112" s="59"/>
+      <c r="Y112" s="59"/>
+      <c r="Z112" s="58" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A113" s="56" t="s">
         <v>83</v>
       </c>
@@ -7337,11 +8003,17 @@
         <v>76.5</v>
       </c>
       <c r="S113" s="59"/>
-      <c r="T113" s="58" t="s">
+      <c r="T113" s="59"/>
+      <c r="U113" s="59"/>
+      <c r="V113" s="59"/>
+      <c r="W113" s="59"/>
+      <c r="X113" s="59"/>
+      <c r="Y113" s="59"/>
+      <c r="Z113" s="58" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A114" s="60" t="s">
         <v>83</v>
       </c>
@@ -7383,13 +8055,21 @@
       <c r="Q114" s="63">
         <v>17</v>
       </c>
-      <c r="R114" s="63"/>
+      <c r="R114" s="63">
+        <v>76.5</v>
+      </c>
       <c r="S114" s="63"/>
-      <c r="T114" s="62" t="s">
+      <c r="T114" s="63"/>
+      <c r="U114" s="63"/>
+      <c r="V114" s="63"/>
+      <c r="W114" s="63"/>
+      <c r="X114" s="63"/>
+      <c r="Y114" s="63"/>
+      <c r="Z114" s="62" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A115" s="34" t="s">
         <v>83</v>
       </c>
@@ -7431,13 +8111,21 @@
       <c r="Q115" s="65">
         <v>17</v>
       </c>
-      <c r="R115" s="65"/>
+      <c r="R115" s="65">
+        <v>76.5</v>
+      </c>
       <c r="S115" s="65"/>
-      <c r="T115" s="34" t="s">
+      <c r="T115" s="65"/>
+      <c r="U115" s="65"/>
+      <c r="V115" s="65"/>
+      <c r="W115" s="65"/>
+      <c r="X115" s="65"/>
+      <c r="Y115" s="65"/>
+      <c r="Z115" s="34" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A116" s="34" t="s">
         <v>83</v>
       </c>
@@ -7479,13 +8167,21 @@
       <c r="Q116" s="65">
         <v>17</v>
       </c>
-      <c r="R116" s="65"/>
+      <c r="R116" s="65">
+        <v>76.5</v>
+      </c>
       <c r="S116" s="65"/>
-      <c r="T116" s="34" t="s">
+      <c r="T116" s="65"/>
+      <c r="U116" s="65"/>
+      <c r="V116" s="65"/>
+      <c r="W116" s="65"/>
+      <c r="X116" s="65"/>
+      <c r="Y116" s="65"/>
+      <c r="Z116" s="34" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A117" s="34" t="s">
         <v>83</v>
       </c>
@@ -7527,13 +8223,21 @@
       <c r="Q117" s="65">
         <v>17</v>
       </c>
-      <c r="R117" s="65"/>
+      <c r="R117" s="65">
+        <v>76.5</v>
+      </c>
       <c r="S117" s="65"/>
-      <c r="T117" s="34" t="s">
+      <c r="T117" s="65"/>
+      <c r="U117" s="65"/>
+      <c r="V117" s="65"/>
+      <c r="W117" s="65"/>
+      <c r="X117" s="65"/>
+      <c r="Y117" s="65"/>
+      <c r="Z117" s="34" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A118" s="66" t="s">
         <v>83</v>
       </c>
@@ -7568,18 +8272,36 @@
       <c r="N118" s="66"/>
       <c r="O118" s="66"/>
       <c r="P118" s="69">
-        <v>0</v>
+        <v>298</v>
       </c>
       <c r="Q118" s="69">
         <v>17</v>
       </c>
-      <c r="R118" s="66"/>
+      <c r="R118" s="66">
+        <v>76.5</v>
+      </c>
       <c r="S118" s="66"/>
       <c r="T118" s="66" t="s">
+        <v>261</v>
+      </c>
+      <c r="U118" s="66">
+        <v>15</v>
+      </c>
+      <c r="V118" s="66"/>
+      <c r="W118" s="66">
+        <v>0</v>
+      </c>
+      <c r="X118" s="66">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Y118" s="66">
+        <v>50</v>
+      </c>
+      <c r="Z118" s="66" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A119" s="66" t="s">
         <v>83</v>
       </c>
@@ -7614,66 +8336,102 @@
       <c r="N119" s="66"/>
       <c r="O119" s="66"/>
       <c r="P119" s="69">
-        <v>0</v>
+        <v>298</v>
       </c>
       <c r="Q119" s="69">
         <v>17</v>
       </c>
-      <c r="R119" s="66"/>
+      <c r="R119" s="66">
+        <v>76.5</v>
+      </c>
       <c r="S119" s="66"/>
       <c r="T119" s="66" t="s">
+        <v>261</v>
+      </c>
+      <c r="U119" s="66">
+        <v>15</v>
+      </c>
+      <c r="V119" s="66"/>
+      <c r="W119" s="66">
+        <v>0</v>
+      </c>
+      <c r="X119" s="66">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Y119" s="66">
+        <v>50</v>
+      </c>
+      <c r="Z119" s="66" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A120" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="B120" s="40"/>
-      <c r="C120" s="40"/>
-      <c r="D120" s="41">
-        <v>43573</v>
-      </c>
-      <c r="E120" s="70" t="s">
-        <v>230</v>
-      </c>
-      <c r="F120" s="40" t="s">
-        <v>231</v>
-      </c>
-      <c r="G120" s="71">
-        <v>1</v>
-      </c>
-      <c r="H120" s="40"/>
-      <c r="I120" s="70" t="s">
-        <v>47</v>
-      </c>
-      <c r="J120" s="71">
-        <v>30</v>
-      </c>
-      <c r="K120" s="71">
-        <v>15</v>
-      </c>
-      <c r="L120" s="70" t="s">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A120" s="66" t="s">
+        <v>83</v>
+      </c>
+      <c r="B120" s="66"/>
+      <c r="C120" s="66"/>
+      <c r="D120" s="67">
+        <v>43570</v>
+      </c>
+      <c r="E120" s="68" t="s">
+        <v>253</v>
+      </c>
+      <c r="F120" s="66" t="s">
+        <v>226</v>
+      </c>
+      <c r="G120" s="69">
+        <v>3</v>
+      </c>
+      <c r="H120" s="66"/>
+      <c r="I120" s="68" t="s">
+        <v>227</v>
+      </c>
+      <c r="J120" s="69">
+        <v>30</v>
+      </c>
+      <c r="K120" s="66"/>
+      <c r="L120" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="M120" s="71">
-        <v>20</v>
-      </c>
-      <c r="N120" s="40"/>
-      <c r="O120" s="40"/>
-      <c r="P120" s="71">
-        <v>873</v>
-      </c>
-      <c r="Q120" s="71">
-        <v>17</v>
-      </c>
-      <c r="R120" s="40"/>
-      <c r="S120" s="40"/>
-      <c r="T120" s="40" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="M120" s="69">
+        <v>30</v>
+      </c>
+      <c r="N120" s="66"/>
+      <c r="O120" s="66"/>
+      <c r="P120" s="69">
+        <v>298</v>
+      </c>
+      <c r="Q120" s="69">
+        <v>17</v>
+      </c>
+      <c r="R120" s="66">
+        <v>76.5</v>
+      </c>
+      <c r="S120" s="66"/>
+      <c r="T120" s="66" t="s">
+        <v>261</v>
+      </c>
+      <c r="U120" s="66">
+        <v>90</v>
+      </c>
+      <c r="V120" s="66" t="s">
+        <v>262</v>
+      </c>
+      <c r="W120" s="66">
+        <v>10</v>
+      </c>
+      <c r="X120" s="66">
+        <v>0.01</v>
+      </c>
+      <c r="Y120" s="66">
+        <v>50</v>
+      </c>
+      <c r="Z120" s="66" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="121" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A121" s="40" t="s">
         <v>83</v>
       </c>
@@ -7683,13 +8441,13 @@
         <v>43573</v>
       </c>
       <c r="E121" s="70" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F121" s="40" t="s">
         <v>231</v>
       </c>
       <c r="G121" s="71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H121" s="40"/>
       <c r="I121" s="70" t="s">
@@ -7705,7 +8463,7 @@
         <v>9</v>
       </c>
       <c r="M121" s="71">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="N121" s="40"/>
       <c r="O121" s="40"/>
@@ -7715,13 +8473,21 @@
       <c r="Q121" s="71">
         <v>17</v>
       </c>
-      <c r="R121" s="40"/>
+      <c r="R121" s="40">
+        <v>76.5</v>
+      </c>
       <c r="S121" s="40"/>
-      <c r="T121" s="40" t="s">
+      <c r="T121" s="40"/>
+      <c r="U121" s="40"/>
+      <c r="V121" s="40"/>
+      <c r="W121" s="40"/>
+      <c r="X121" s="40"/>
+      <c r="Y121" s="40"/>
+      <c r="Z121" s="40" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A122" s="40" t="s">
         <v>83</v>
       </c>
@@ -7731,13 +8497,13 @@
         <v>43573</v>
       </c>
       <c r="E122" s="70" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F122" s="40" t="s">
         <v>231</v>
       </c>
       <c r="G122" s="71">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H122" s="40"/>
       <c r="I122" s="70" t="s">
@@ -7753,7 +8519,7 @@
         <v>9</v>
       </c>
       <c r="M122" s="71">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="N122" s="40"/>
       <c r="O122" s="40"/>
@@ -7763,13 +8529,21 @@
       <c r="Q122" s="71">
         <v>17</v>
       </c>
-      <c r="R122" s="40"/>
+      <c r="R122" s="40">
+        <v>76.5</v>
+      </c>
       <c r="S122" s="40"/>
-      <c r="T122" s="40" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T122" s="40"/>
+      <c r="U122" s="40"/>
+      <c r="V122" s="40"/>
+      <c r="W122" s="40"/>
+      <c r="X122" s="40"/>
+      <c r="Y122" s="40"/>
+      <c r="Z122" s="40" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="123" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A123" s="40" t="s">
         <v>83</v>
       </c>
@@ -7779,13 +8553,13 @@
         <v>43573</v>
       </c>
       <c r="E123" s="70" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F123" s="40" t="s">
         <v>231</v>
       </c>
       <c r="G123" s="71">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H123" s="40"/>
       <c r="I123" s="70" t="s">
@@ -7801,7 +8575,7 @@
         <v>9</v>
       </c>
       <c r="M123" s="71">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="N123" s="40"/>
       <c r="O123" s="40"/>
@@ -7811,61 +8585,77 @@
       <c r="Q123" s="71">
         <v>17</v>
       </c>
-      <c r="R123" s="40"/>
+      <c r="R123" s="40">
+        <v>76.5</v>
+      </c>
       <c r="S123" s="40"/>
-      <c r="T123" s="40" t="s">
+      <c r="T123" s="40"/>
+      <c r="U123" s="40"/>
+      <c r="V123" s="40"/>
+      <c r="W123" s="40"/>
+      <c r="X123" s="40"/>
+      <c r="Y123" s="40"/>
+      <c r="Z123" s="40" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="124" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A124" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B124" s="40"/>
+      <c r="C124" s="40"/>
+      <c r="D124" s="41">
+        <v>43573</v>
+      </c>
+      <c r="E124" s="70" t="s">
+        <v>235</v>
+      </c>
+      <c r="F124" s="40" t="s">
+        <v>231</v>
+      </c>
+      <c r="G124" s="71">
+        <v>4</v>
+      </c>
+      <c r="H124" s="40"/>
+      <c r="I124" s="70" t="s">
+        <v>47</v>
+      </c>
+      <c r="J124" s="71">
+        <v>30</v>
+      </c>
+      <c r="K124" s="71">
+        <v>15</v>
+      </c>
+      <c r="L124" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="M124" s="71">
+        <v>60</v>
+      </c>
+      <c r="N124" s="40"/>
+      <c r="O124" s="40"/>
+      <c r="P124" s="71">
+        <v>873</v>
+      </c>
+      <c r="Q124" s="71">
+        <v>17</v>
+      </c>
+      <c r="R124" s="40">
+        <v>76.5</v>
+      </c>
+      <c r="S124" s="40"/>
+      <c r="T124" s="40"/>
+      <c r="U124" s="40"/>
+      <c r="V124" s="40"/>
+      <c r="W124" s="40"/>
+      <c r="X124" s="40"/>
+      <c r="Y124" s="40"/>
+      <c r="Z124" s="40" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A124" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="B124" s="47"/>
-      <c r="C124" s="47"/>
-      <c r="D124" s="48">
-        <v>43580</v>
-      </c>
-      <c r="E124" s="72" t="s">
-        <v>238</v>
-      </c>
-      <c r="F124" s="47" t="s">
-        <v>239</v>
-      </c>
-      <c r="G124" s="50">
-        <v>1</v>
-      </c>
-      <c r="H124" s="47"/>
-      <c r="I124" s="72" t="s">
-        <v>47</v>
-      </c>
-      <c r="J124" s="50">
-        <v>5</v>
-      </c>
-      <c r="K124" s="50">
-        <v>15</v>
-      </c>
-      <c r="L124" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="M124" s="50">
-        <v>30</v>
-      </c>
-      <c r="N124" s="47"/>
-      <c r="O124" s="47"/>
-      <c r="P124" s="50">
-        <v>0</v>
-      </c>
-      <c r="Q124" s="50">
-        <v>17</v>
-      </c>
-      <c r="R124" s="47"/>
-      <c r="S124" s="47"/>
-      <c r="T124" s="47" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A125" s="47" t="s">
         <v>83</v>
       </c>
@@ -7875,13 +8665,13 @@
         <v>43580</v>
       </c>
       <c r="E125" s="72" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="F125" s="47" t="s">
         <v>239</v>
       </c>
       <c r="G125" s="50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H125" s="47"/>
       <c r="I125" s="72" t="s">
@@ -7902,34 +8692,42 @@
       <c r="N125" s="47"/>
       <c r="O125" s="47"/>
       <c r="P125" s="50">
-        <v>873</v>
+        <v>0</v>
       </c>
       <c r="Q125" s="50">
         <v>17</v>
       </c>
-      <c r="R125" s="47"/>
+      <c r="R125" s="47">
+        <v>76.5</v>
+      </c>
       <c r="S125" s="47"/>
-      <c r="T125" s="47" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T125" s="47"/>
+      <c r="U125" s="47"/>
+      <c r="V125" s="47"/>
+      <c r="W125" s="47"/>
+      <c r="X125" s="47"/>
+      <c r="Y125" s="47"/>
+      <c r="Z125" s="47" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="126" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A126" s="47" t="s">
         <v>83</v>
       </c>
       <c r="B126" s="47"/>
       <c r="C126" s="47"/>
       <c r="D126" s="48">
-        <v>43581</v>
+        <v>43580</v>
       </c>
       <c r="E126" s="72" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="F126" s="47" t="s">
         <v>239</v>
       </c>
       <c r="G126" s="50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H126" s="47"/>
       <c r="I126" s="72" t="s">
@@ -7955,69 +8753,93 @@
       <c r="Q126" s="50">
         <v>17</v>
       </c>
-      <c r="R126" s="47"/>
+      <c r="R126" s="47">
+        <v>76.5</v>
+      </c>
       <c r="S126" s="47"/>
-      <c r="T126" s="47" t="s">
+      <c r="T126" s="47"/>
+      <c r="U126" s="47"/>
+      <c r="V126" s="47"/>
+      <c r="W126" s="47"/>
+      <c r="X126" s="47"/>
+      <c r="Y126" s="47"/>
+      <c r="Z126" s="47" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="127" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A127" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B127" s="47"/>
+      <c r="C127" s="47"/>
+      <c r="D127" s="48">
+        <v>43581</v>
+      </c>
+      <c r="E127" s="72" t="s">
+        <v>243</v>
+      </c>
+      <c r="F127" s="47" t="s">
+        <v>239</v>
+      </c>
+      <c r="G127" s="50">
+        <v>3</v>
+      </c>
+      <c r="H127" s="47"/>
+      <c r="I127" s="72" t="s">
+        <v>47</v>
+      </c>
+      <c r="J127" s="50">
+        <v>5</v>
+      </c>
+      <c r="K127" s="50">
+        <v>15</v>
+      </c>
+      <c r="L127" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="M127" s="50">
+        <v>30</v>
+      </c>
+      <c r="N127" s="47"/>
+      <c r="O127" s="47"/>
+      <c r="P127" s="50">
+        <v>873</v>
+      </c>
+      <c r="Q127" s="50">
+        <v>17</v>
+      </c>
+      <c r="R127" s="47">
+        <v>76.5</v>
+      </c>
+      <c r="S127" s="47"/>
+      <c r="T127" s="47"/>
+      <c r="U127" s="47"/>
+      <c r="V127" s="47"/>
+      <c r="W127" s="47"/>
+      <c r="X127" s="47"/>
+      <c r="Y127" s="47"/>
+      <c r="Z127" s="47" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A127" s="60" t="s">
-        <v>83</v>
-      </c>
-      <c r="B127" s="60"/>
-      <c r="C127" s="60"/>
-      <c r="D127" s="61">
-        <v>43581</v>
-      </c>
-      <c r="E127" s="62" t="s">
-        <v>245</v>
-      </c>
-      <c r="F127" s="60" t="s">
-        <v>246</v>
-      </c>
-      <c r="G127" s="63">
-        <v>1</v>
-      </c>
-      <c r="H127" s="60"/>
-      <c r="I127" s="62" t="s">
-        <v>9</v>
-      </c>
-      <c r="J127" s="63">
-        <v>30</v>
-      </c>
-      <c r="K127" s="60"/>
-      <c r="L127" s="60"/>
-      <c r="M127" s="60"/>
-      <c r="N127" s="60"/>
-      <c r="O127" s="60"/>
-      <c r="P127" s="60"/>
-      <c r="Q127" s="63">
-        <v>17</v>
-      </c>
-      <c r="R127" s="60"/>
-      <c r="S127" s="60"/>
-      <c r="T127" s="60" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A128" s="60" t="s">
         <v>83</v>
       </c>
       <c r="B128" s="60"/>
       <c r="C128" s="60"/>
       <c r="D128" s="61">
-        <v>43608</v>
+        <v>43581</v>
       </c>
       <c r="E128" s="62" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="F128" s="60" t="s">
         <v>246</v>
       </c>
       <c r="G128" s="63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H128" s="60"/>
       <c r="I128" s="62" t="s">
@@ -8035,29 +8857,37 @@
       <c r="Q128" s="63">
         <v>17</v>
       </c>
-      <c r="R128" s="60"/>
+      <c r="R128" s="60">
+        <v>76.5</v>
+      </c>
       <c r="S128" s="60"/>
-      <c r="T128" s="60" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T128" s="60"/>
+      <c r="U128" s="60"/>
+      <c r="V128" s="60"/>
+      <c r="W128" s="60"/>
+      <c r="X128" s="60"/>
+      <c r="Y128" s="60"/>
+      <c r="Z128" s="60" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="129" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A129" s="60" t="s">
         <v>83</v>
       </c>
       <c r="B129" s="60"/>
       <c r="C129" s="60"/>
       <c r="D129" s="61">
-        <v>43609</v>
+        <v>43608</v>
       </c>
       <c r="E129" s="62" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F129" s="60" t="s">
         <v>246</v>
       </c>
       <c r="G129" s="63">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H129" s="60"/>
       <c r="I129" s="62" t="s">
@@ -8075,9 +8905,65 @@
       <c r="Q129" s="63">
         <v>17</v>
       </c>
-      <c r="R129" s="60"/>
+      <c r="R129" s="60">
+        <v>76.5</v>
+      </c>
       <c r="S129" s="60"/>
-      <c r="T129" s="60" t="s">
+      <c r="T129" s="60"/>
+      <c r="U129" s="60"/>
+      <c r="V129" s="60"/>
+      <c r="W129" s="60"/>
+      <c r="X129" s="60"/>
+      <c r="Y129" s="60"/>
+      <c r="Z129" s="60" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="130" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A130" s="60" t="s">
+        <v>83</v>
+      </c>
+      <c r="B130" s="60"/>
+      <c r="C130" s="60"/>
+      <c r="D130" s="61">
+        <v>43609</v>
+      </c>
+      <c r="E130" s="62" t="s">
+        <v>249</v>
+      </c>
+      <c r="F130" s="60" t="s">
+        <v>246</v>
+      </c>
+      <c r="G130" s="63">
+        <v>3</v>
+      </c>
+      <c r="H130" s="60"/>
+      <c r="I130" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="J130" s="63">
+        <v>30</v>
+      </c>
+      <c r="K130" s="60"/>
+      <c r="L130" s="60"/>
+      <c r="M130" s="60"/>
+      <c r="N130" s="60"/>
+      <c r="O130" s="60"/>
+      <c r="P130" s="60"/>
+      <c r="Q130" s="63">
+        <v>17</v>
+      </c>
+      <c r="R130" s="60">
+        <v>76.5</v>
+      </c>
+      <c r="S130" s="60"/>
+      <c r="T130" s="60"/>
+      <c r="U130" s="60"/>
+      <c r="V130" s="60"/>
+      <c r="W130" s="60"/>
+      <c r="X130" s="60"/>
+      <c r="Y130" s="60"/>
+      <c r="Z130" s="60" t="s">
         <v>252</v>
       </c>
     </row>
@@ -8095,7 +8981,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>

</xml_diff>

<commit_message>
Can load just the sample table
</commit_message>
<xml_diff>
--- a/ivtools/sampledata/CeRAM_Depositions.xlsx
+++ b/ivtools/sampledata/CeRAM_Depositions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\t\py-ivtools\ivtools\sampledata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\emrl\Pool\Projekte\HGST-CERAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="271">
   <si>
     <t>wafer_number</t>
   </si>
@@ -809,12 +809,36 @@
   </si>
   <si>
     <t>1%O2/99%Ar</t>
+  </si>
+  <si>
+    <t>Hund1</t>
+  </si>
+  <si>
+    <t>NVM303_0262</t>
+  </si>
+  <si>
+    <t>DomeB</t>
+  </si>
+  <si>
+    <t>Hund</t>
+  </si>
+  <si>
+    <t>NVM303_0091</t>
+  </si>
+  <si>
+    <t>Hund2</t>
+  </si>
+  <si>
+    <t>first test of new wafers, 30nm amorphous (VCr15)2O3 nominal on 50nm TaN wafer</t>
+  </si>
+  <si>
+    <t>second test of new wafers, 30nm amorphous (VCr15)2O3 nominal on 25 nm TiN wafer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -957,7 +981,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="56">
+  <fills count="57">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1275,6 +1299,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1436,7 +1466,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1518,50 +1548,54 @@
     <xf numFmtId="2" fontId="0" fillId="49" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="49" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="52" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1844,18 +1878,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z130"/>
+  <dimension ref="A1:Z132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V119" sqref="V119"/>
+      <pane ySplit="9" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z133" sqref="Z133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
@@ -8967,6 +9001,130 @@
         <v>252</v>
       </c>
     </row>
+    <row r="131" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A131" s="73" t="s">
+        <v>265</v>
+      </c>
+      <c r="B131" s="73" t="s">
+        <v>264</v>
+      </c>
+      <c r="C131" s="73"/>
+      <c r="D131" s="74">
+        <v>43713</v>
+      </c>
+      <c r="E131" s="75" t="s">
+        <v>263</v>
+      </c>
+      <c r="F131" s="75" t="s">
+        <v>266</v>
+      </c>
+      <c r="G131" s="76">
+        <v>1</v>
+      </c>
+      <c r="H131" s="73"/>
+      <c r="I131" s="75" t="s">
+        <v>47</v>
+      </c>
+      <c r="J131" s="76">
+        <v>30</v>
+      </c>
+      <c r="K131" s="73">
+        <v>15</v>
+      </c>
+      <c r="L131" s="73"/>
+      <c r="M131" s="73"/>
+      <c r="N131" s="73"/>
+      <c r="O131" s="73"/>
+      <c r="P131" s="76">
+        <v>298</v>
+      </c>
+      <c r="Q131" s="76"/>
+      <c r="R131" s="73"/>
+      <c r="S131" s="73"/>
+      <c r="T131" s="73" t="s">
+        <v>261</v>
+      </c>
+      <c r="U131" s="73">
+        <v>98</v>
+      </c>
+      <c r="V131" s="73" t="s">
+        <v>262</v>
+      </c>
+      <c r="W131" s="73">
+        <v>6</v>
+      </c>
+      <c r="X131" s="73">
+        <v>0.01</v>
+      </c>
+      <c r="Y131" s="73">
+        <v>50</v>
+      </c>
+      <c r="Z131" s="73" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="132" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A132" s="73" t="s">
+        <v>265</v>
+      </c>
+      <c r="B132" s="73" t="s">
+        <v>267</v>
+      </c>
+      <c r="C132" s="73"/>
+      <c r="D132" s="74">
+        <v>43713</v>
+      </c>
+      <c r="E132" s="75" t="s">
+        <v>268</v>
+      </c>
+      <c r="F132" s="75" t="s">
+        <v>266</v>
+      </c>
+      <c r="G132" s="76">
+        <v>2</v>
+      </c>
+      <c r="H132" s="73"/>
+      <c r="I132" s="75" t="s">
+        <v>47</v>
+      </c>
+      <c r="J132" s="76">
+        <v>30</v>
+      </c>
+      <c r="K132" s="73">
+        <v>15</v>
+      </c>
+      <c r="L132" s="73"/>
+      <c r="M132" s="73"/>
+      <c r="N132" s="73"/>
+      <c r="O132" s="73"/>
+      <c r="P132" s="76">
+        <v>298</v>
+      </c>
+      <c r="Q132" s="76"/>
+      <c r="R132" s="73"/>
+      <c r="S132" s="73"/>
+      <c r="T132" s="73" t="s">
+        <v>261</v>
+      </c>
+      <c r="U132" s="73">
+        <v>98</v>
+      </c>
+      <c r="V132" s="73" t="s">
+        <v>262</v>
+      </c>
+      <c r="W132" s="73">
+        <v>6</v>
+      </c>
+      <c r="X132" s="73">
+        <v>0.01</v>
+      </c>
+      <c r="Y132" s="73">
+        <v>50</v>
+      </c>
+      <c r="Z132" s="73" t="s">
+        <v>270</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8981,7 +9139,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>

</xml_diff>

<commit_message>
resistance() doesn't crash with np.nan
</commit_message>
<xml_diff>
--- a/ivtools/sampledata/CeRAM_Depositions.xlsx
+++ b/ivtools/sampledata/CeRAM_Depositions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="280">
   <si>
     <t>wafer_number</t>
   </si>
@@ -833,12 +833,39 @@
   </si>
   <si>
     <t>second test of new wafers, 30nm amorphous (VCr15)2O3 nominal on 25 nm TiN wafer</t>
+  </si>
+  <si>
+    <t>Hund3</t>
+  </si>
+  <si>
+    <t>30nm V2O3 nominal, seems to be VO2; film thickness could be off</t>
+  </si>
+  <si>
+    <t>Esel1</t>
+  </si>
+  <si>
+    <t>Esel</t>
+  </si>
+  <si>
+    <t>Esel5</t>
+  </si>
+  <si>
+    <t>Esel4</t>
+  </si>
+  <si>
+    <t>Esel3</t>
+  </si>
+  <si>
+    <t>Esel2</t>
+  </si>
+  <si>
+    <t>new (VCr15)2O3 thickness series</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -981,7 +1008,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="57">
+  <fills count="58">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1305,6 +1332,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1466,7 +1499,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1552,50 +1585,54 @@
     <xf numFmtId="14" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="56" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="57" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="57" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="57" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="57" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1878,14 +1915,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z132"/>
+  <dimension ref="A1:Z138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z133" sqref="Z133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B134" sqref="B134"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -9045,7 +9082,7 @@
         <v>261</v>
       </c>
       <c r="U131" s="73">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="V131" s="73" t="s">
         <v>262</v>
@@ -9107,7 +9144,7 @@
         <v>261</v>
       </c>
       <c r="U132" s="73">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="V132" s="73" t="s">
         <v>262</v>
@@ -9123,6 +9160,424 @@
       </c>
       <c r="Z132" s="73" t="s">
         <v>270</v>
+      </c>
+    </row>
+    <row r="133" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A133" s="73" t="s">
+        <v>265</v>
+      </c>
+      <c r="B133" s="73" t="s">
+        <v>267</v>
+      </c>
+      <c r="C133" s="73"/>
+      <c r="D133" s="74">
+        <v>43726</v>
+      </c>
+      <c r="E133" s="75" t="s">
+        <v>271</v>
+      </c>
+      <c r="F133" s="75" t="s">
+        <v>266</v>
+      </c>
+      <c r="G133" s="76">
+        <v>3</v>
+      </c>
+      <c r="H133" s="73"/>
+      <c r="I133" s="75" t="s">
+        <v>186</v>
+      </c>
+      <c r="J133" s="76">
+        <v>30</v>
+      </c>
+      <c r="K133" s="73"/>
+      <c r="L133" s="73"/>
+      <c r="M133" s="73"/>
+      <c r="N133" s="73"/>
+      <c r="O133" s="73"/>
+      <c r="P133" s="76">
+        <v>298</v>
+      </c>
+      <c r="Q133" s="76"/>
+      <c r="R133" s="73"/>
+      <c r="S133" s="73">
+        <v>1073</v>
+      </c>
+      <c r="T133" s="73" t="s">
+        <v>261</v>
+      </c>
+      <c r="U133" s="73">
+        <v>94</v>
+      </c>
+      <c r="V133" s="73" t="s">
+        <v>262</v>
+      </c>
+      <c r="W133" s="73">
+        <v>6</v>
+      </c>
+      <c r="X133" s="73">
+        <v>0.01</v>
+      </c>
+      <c r="Y133" s="73">
+        <v>50</v>
+      </c>
+      <c r="Z133" s="73" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="134" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A134" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="B134" s="77">
+        <v>21519</v>
+      </c>
+      <c r="C134" s="77">
+        <v>2</v>
+      </c>
+      <c r="D134" s="78">
+        <v>43739</v>
+      </c>
+      <c r="E134" s="79" t="s">
+        <v>273</v>
+      </c>
+      <c r="F134" s="79" t="s">
+        <v>274</v>
+      </c>
+      <c r="G134" s="80">
+        <v>1</v>
+      </c>
+      <c r="H134" s="77"/>
+      <c r="I134" s="79" t="s">
+        <v>47</v>
+      </c>
+      <c r="J134" s="80">
+        <v>10</v>
+      </c>
+      <c r="K134" s="77">
+        <v>15</v>
+      </c>
+      <c r="L134" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="M134" s="77">
+        <v>30</v>
+      </c>
+      <c r="N134" s="77"/>
+      <c r="O134" s="77"/>
+      <c r="P134" s="80">
+        <v>873</v>
+      </c>
+      <c r="Q134" s="80">
+        <v>17</v>
+      </c>
+      <c r="R134" s="77">
+        <v>76.5</v>
+      </c>
+      <c r="S134" s="77"/>
+      <c r="T134" s="77" t="s">
+        <v>261</v>
+      </c>
+      <c r="U134" s="77">
+        <v>94</v>
+      </c>
+      <c r="V134" s="77" t="s">
+        <v>262</v>
+      </c>
+      <c r="W134" s="77">
+        <v>6</v>
+      </c>
+      <c r="X134" s="77">
+        <v>0.01</v>
+      </c>
+      <c r="Y134" s="77">
+        <v>50</v>
+      </c>
+      <c r="Z134" s="77" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="135" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A135" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="B135" s="77">
+        <v>21519</v>
+      </c>
+      <c r="C135" s="77">
+        <v>4</v>
+      </c>
+      <c r="D135" s="78">
+        <v>43739</v>
+      </c>
+      <c r="E135" s="79" t="s">
+        <v>278</v>
+      </c>
+      <c r="F135" s="79" t="s">
+        <v>274</v>
+      </c>
+      <c r="G135" s="80">
+        <v>2</v>
+      </c>
+      <c r="H135" s="77"/>
+      <c r="I135" s="79" t="s">
+        <v>47</v>
+      </c>
+      <c r="J135" s="80">
+        <v>5</v>
+      </c>
+      <c r="K135" s="77">
+        <v>15</v>
+      </c>
+      <c r="L135" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="M135" s="77">
+        <v>30</v>
+      </c>
+      <c r="N135" s="77"/>
+      <c r="O135" s="77"/>
+      <c r="P135" s="80">
+        <v>873</v>
+      </c>
+      <c r="Q135" s="80">
+        <v>17</v>
+      </c>
+      <c r="R135" s="77">
+        <v>76.5</v>
+      </c>
+      <c r="S135" s="77"/>
+      <c r="T135" s="77" t="s">
+        <v>261</v>
+      </c>
+      <c r="U135" s="77">
+        <v>94</v>
+      </c>
+      <c r="V135" s="77" t="s">
+        <v>262</v>
+      </c>
+      <c r="W135" s="77">
+        <v>6</v>
+      </c>
+      <c r="X135" s="77">
+        <v>0.01</v>
+      </c>
+      <c r="Y135" s="77">
+        <v>50</v>
+      </c>
+      <c r="Z135" s="77" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="136" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A136" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="B136" s="77">
+        <v>21519</v>
+      </c>
+      <c r="C136" s="77">
+        <v>3</v>
+      </c>
+      <c r="D136" s="78">
+        <v>43739</v>
+      </c>
+      <c r="E136" s="79" t="s">
+        <v>277</v>
+      </c>
+      <c r="F136" s="79" t="s">
+        <v>274</v>
+      </c>
+      <c r="G136" s="80">
+        <v>3</v>
+      </c>
+      <c r="H136" s="77"/>
+      <c r="I136" s="79" t="s">
+        <v>47</v>
+      </c>
+      <c r="J136" s="80">
+        <v>30</v>
+      </c>
+      <c r="K136" s="77">
+        <v>15</v>
+      </c>
+      <c r="L136" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="M136" s="77">
+        <v>30</v>
+      </c>
+      <c r="N136" s="77"/>
+      <c r="O136" s="77"/>
+      <c r="P136" s="80">
+        <v>873</v>
+      </c>
+      <c r="Q136" s="80">
+        <v>17</v>
+      </c>
+      <c r="R136" s="77">
+        <v>76.5</v>
+      </c>
+      <c r="S136" s="77"/>
+      <c r="T136" s="77" t="s">
+        <v>261</v>
+      </c>
+      <c r="U136" s="77">
+        <v>94</v>
+      </c>
+      <c r="V136" s="77" t="s">
+        <v>262</v>
+      </c>
+      <c r="W136" s="77">
+        <v>6</v>
+      </c>
+      <c r="X136" s="77">
+        <v>0.01</v>
+      </c>
+      <c r="Y136" s="77">
+        <v>50</v>
+      </c>
+      <c r="Z136" s="77" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="137" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A137" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="B137" s="77">
+        <v>21519</v>
+      </c>
+      <c r="C137" s="77">
+        <v>5</v>
+      </c>
+      <c r="D137" s="78">
+        <v>43739</v>
+      </c>
+      <c r="E137" s="79" t="s">
+        <v>276</v>
+      </c>
+      <c r="F137" s="79" t="s">
+        <v>274</v>
+      </c>
+      <c r="G137" s="80">
+        <v>4</v>
+      </c>
+      <c r="H137" s="77"/>
+      <c r="I137" s="79" t="s">
+        <v>47</v>
+      </c>
+      <c r="J137" s="80">
+        <v>20</v>
+      </c>
+      <c r="K137" s="77">
+        <v>15</v>
+      </c>
+      <c r="L137" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="M137" s="77">
+        <v>30</v>
+      </c>
+      <c r="N137" s="77"/>
+      <c r="O137" s="77"/>
+      <c r="P137" s="80">
+        <v>873</v>
+      </c>
+      <c r="Q137" s="80">
+        <v>17</v>
+      </c>
+      <c r="R137" s="77">
+        <v>76.5</v>
+      </c>
+      <c r="S137" s="77"/>
+      <c r="T137" s="77" t="s">
+        <v>261</v>
+      </c>
+      <c r="U137" s="77">
+        <v>94</v>
+      </c>
+      <c r="V137" s="77" t="s">
+        <v>262</v>
+      </c>
+      <c r="W137" s="77">
+        <v>6</v>
+      </c>
+      <c r="X137" s="77">
+        <v>0.01</v>
+      </c>
+      <c r="Y137" s="77">
+        <v>50</v>
+      </c>
+      <c r="Z137" s="77" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="138" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A138" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="B138" s="77">
+        <v>21519</v>
+      </c>
+      <c r="C138" s="77">
+        <v>1</v>
+      </c>
+      <c r="D138" s="78">
+        <v>43739</v>
+      </c>
+      <c r="E138" s="79" t="s">
+        <v>275</v>
+      </c>
+      <c r="F138" s="79" t="s">
+        <v>274</v>
+      </c>
+      <c r="G138" s="80">
+        <v>5</v>
+      </c>
+      <c r="H138" s="77"/>
+      <c r="I138" s="77" t="s">
+        <v>9</v>
+      </c>
+      <c r="J138" s="80">
+        <v>30</v>
+      </c>
+      <c r="K138" s="77">
+        <v>15</v>
+      </c>
+      <c r="L138" s="77"/>
+      <c r="M138" s="77"/>
+      <c r="N138" s="77"/>
+      <c r="O138" s="77"/>
+      <c r="P138" s="80">
+        <v>873</v>
+      </c>
+      <c r="Q138" s="80">
+        <v>17</v>
+      </c>
+      <c r="R138" s="77">
+        <v>76.5</v>
+      </c>
+      <c r="S138" s="77"/>
+      <c r="T138" s="77" t="s">
+        <v>261</v>
+      </c>
+      <c r="U138" s="77">
+        <v>94</v>
+      </c>
+      <c r="V138" s="77" t="s">
+        <v>262</v>
+      </c>
+      <c r="W138" s="77">
+        <v>6</v>
+      </c>
+      <c r="X138" s="77">
+        <v>0.01</v>
+      </c>
+      <c r="Y138" s="77">
+        <v>50</v>
+      </c>
+      <c r="Z138" s="77" t="s">
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -9139,7 +9594,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>

</xml_diff>

<commit_message>
I updated pico-python to save the channel couplings, then updated Picoscope to use them
</commit_message>
<xml_diff>
--- a/ivtools/sampledata/CeRAM_Depositions.xlsx
+++ b/ivtools/sampledata/CeRAM_Depositions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="294">
   <si>
     <t>wafer_number</t>
   </si>
@@ -893,6 +893,15 @@
   </si>
   <si>
     <t>used lower ignition power (30W), was not etched</t>
+  </si>
+  <si>
+    <t>Maulesel1</t>
+  </si>
+  <si>
+    <t>Maulesel</t>
+  </si>
+  <si>
+    <t>was etched</t>
   </si>
 </sst>
 </file>
@@ -1538,7 +1547,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1632,6 +1641,8 @@
     <xf numFmtId="14" fontId="0" fillId="58" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="58" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="58" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1958,11 +1969,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z143"/>
+  <dimension ref="A1:Z144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C143" sqref="C143"/>
+      <selection pane="bottomLeft" activeCell="Z134" sqref="Z134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9889,6 +9900,54 @@
         <v>290</v>
       </c>
     </row>
+    <row r="144" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A144" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B144" s="22">
+        <v>21519</v>
+      </c>
+      <c r="C144" s="22">
+        <v>14</v>
+      </c>
+      <c r="D144" s="23">
+        <v>43748</v>
+      </c>
+      <c r="E144" s="85" t="s">
+        <v>291</v>
+      </c>
+      <c r="F144" s="85" t="s">
+        <v>292</v>
+      </c>
+      <c r="G144" s="86">
+        <v>1</v>
+      </c>
+      <c r="H144" s="22"/>
+      <c r="I144" s="85" t="s">
+        <v>9</v>
+      </c>
+      <c r="J144" s="86">
+        <v>30</v>
+      </c>
+      <c r="K144" s="22"/>
+      <c r="L144" s="22"/>
+      <c r="M144" s="22"/>
+      <c r="N144" s="22"/>
+      <c r="O144" s="22"/>
+      <c r="P144" s="22"/>
+      <c r="Q144" s="22"/>
+      <c r="R144" s="22"/>
+      <c r="S144" s="22"/>
+      <c r="T144" s="22"/>
+      <c r="U144" s="22"/>
+      <c r="V144" s="22"/>
+      <c r="W144" s="22"/>
+      <c r="X144" s="22"/>
+      <c r="Y144" s="22"/>
+      <c r="Z144" s="22" t="s">
+        <v>293</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
make static resistance plotter accept multiple loops
</commit_message>
<xml_diff>
--- a/ivtools/sampledata/CeRAM_Depositions.xlsx
+++ b/ivtools/sampledata/CeRAM_Depositions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22980" windowHeight="8280"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="deposition_plan" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="298">
   <si>
     <t>wafer_number</t>
   </si>
@@ -901,10 +901,19 @@
     <t>Maulesel</t>
   </si>
   <si>
-    <t>was etched</t>
-  </si>
-  <si>
     <t>Maulesel2</t>
+  </si>
+  <si>
+    <t>Troubleshooting O2 contamination.  Flushed the CT1000</t>
+  </si>
+  <si>
+    <t>Troubleshooting O2 contamination.  Flushed the etch tool.</t>
+  </si>
+  <si>
+    <t>Maulesel3</t>
+  </si>
+  <si>
+    <t>Troubleshooting O2 contamination.  Flushed everything some more.</t>
   </si>
 </sst>
 </file>
@@ -1972,11 +1981,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z145"/>
+  <dimension ref="A1:Z146"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AA145" sqref="AA145"/>
+      <selection pane="bottomLeft" activeCell="Z147" sqref="Z147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9842,7 +9851,9 @@
       <c r="N142" s="81"/>
       <c r="O142" s="81"/>
       <c r="P142" s="81"/>
-      <c r="Q142" s="81"/>
+      <c r="Q142" s="81">
+        <v>17</v>
+      </c>
       <c r="R142" s="81"/>
       <c r="S142" s="81"/>
       <c r="T142" s="81"/>
@@ -9890,7 +9901,9 @@
       <c r="N143" s="81"/>
       <c r="O143" s="81"/>
       <c r="P143" s="81"/>
-      <c r="Q143" s="81"/>
+      <c r="Q143" s="81">
+        <v>0</v>
+      </c>
       <c r="R143" s="81"/>
       <c r="S143" s="81"/>
       <c r="T143" s="81"/>
@@ -9938,7 +9951,9 @@
       <c r="N144" s="22"/>
       <c r="O144" s="22"/>
       <c r="P144" s="22"/>
-      <c r="Q144" s="22"/>
+      <c r="Q144" s="22">
+        <v>17</v>
+      </c>
       <c r="R144" s="22"/>
       <c r="S144" s="22"/>
       <c r="T144" s="22"/>
@@ -9948,7 +9963,7 @@
       <c r="X144" s="22"/>
       <c r="Y144" s="22"/>
       <c r="Z144" s="22" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="145" spans="1:26" x14ac:dyDescent="0.25">
@@ -9965,7 +9980,7 @@
         <v>43748</v>
       </c>
       <c r="E145" s="85" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F145" s="85" t="s">
         <v>292</v>
@@ -9986,7 +10001,9 @@
       <c r="N145" s="22"/>
       <c r="O145" s="22"/>
       <c r="P145" s="22"/>
-      <c r="Q145" s="22"/>
+      <c r="Q145" s="22">
+        <v>17</v>
+      </c>
       <c r="R145" s="22"/>
       <c r="S145" s="22"/>
       <c r="T145" s="22"/>
@@ -9996,7 +10013,57 @@
       <c r="X145" s="22"/>
       <c r="Y145" s="22"/>
       <c r="Z145" s="22" t="s">
-        <v>293</v>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="146" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A146" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B146" s="22">
+        <v>21519</v>
+      </c>
+      <c r="C146" s="22">
+        <v>10</v>
+      </c>
+      <c r="D146" s="23">
+        <v>43748</v>
+      </c>
+      <c r="E146" s="85" t="s">
+        <v>296</v>
+      </c>
+      <c r="F146" s="85" t="s">
+        <v>292</v>
+      </c>
+      <c r="G146" s="86">
+        <v>3</v>
+      </c>
+      <c r="H146" s="22"/>
+      <c r="I146" s="85" t="s">
+        <v>9</v>
+      </c>
+      <c r="J146" s="86">
+        <v>30</v>
+      </c>
+      <c r="K146" s="22"/>
+      <c r="L146" s="22"/>
+      <c r="M146" s="22"/>
+      <c r="N146" s="22"/>
+      <c r="O146" s="22"/>
+      <c r="P146" s="22"/>
+      <c r="Q146" s="22">
+        <v>17</v>
+      </c>
+      <c r="R146" s="22"/>
+      <c r="S146" s="22"/>
+      <c r="T146" s="22"/>
+      <c r="U146" s="22"/>
+      <c r="V146" s="22"/>
+      <c r="W146" s="22"/>
+      <c r="X146" s="22"/>
+      <c r="Y146" s="22"/>
+      <c r="Z146" s="22" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a bunch of keithley 2600 commands
</commit_message>
<xml_diff>
--- a/ivtools/sampledata/CeRAM_Depositions.xlsx
+++ b/ivtools/sampledata/CeRAM_Depositions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20505" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="deposition_plan" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="306">
   <si>
     <t>wafer_number</t>
   </si>
@@ -932,12 +932,18 @@
   </si>
   <si>
     <t>Murmeltier1</t>
+  </si>
+  <si>
+    <t>Murmeltier2</t>
+  </si>
+  <si>
+    <t>contact test on new wafer with Pt from CS500 deposition tool</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1677,48 +1683,48 @@
     <xf numFmtId="2" fontId="0" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2001,14 +2007,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z148"/>
+  <dimension ref="A1:Z149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H149" sqref="H149"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -10182,6 +10188,52 @@
         <v>301</v>
       </c>
     </row>
+    <row r="149" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A149" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B149" s="87" t="s">
+        <v>300</v>
+      </c>
+      <c r="C149" s="45"/>
+      <c r="D149" s="46">
+        <v>43784</v>
+      </c>
+      <c r="E149" s="45" t="s">
+        <v>304</v>
+      </c>
+      <c r="F149" s="45" t="s">
+        <v>302</v>
+      </c>
+      <c r="G149" s="49">
+        <v>2</v>
+      </c>
+      <c r="H149" s="45"/>
+      <c r="I149" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="J149" s="49">
+        <v>30</v>
+      </c>
+      <c r="K149" s="45"/>
+      <c r="L149" s="45"/>
+      <c r="M149" s="45"/>
+      <c r="N149" s="45"/>
+      <c r="O149" s="45"/>
+      <c r="P149" s="45"/>
+      <c r="Q149" s="45"/>
+      <c r="R149" s="45"/>
+      <c r="S149" s="45"/>
+      <c r="T149" s="45"/>
+      <c r="U149" s="45"/>
+      <c r="V149" s="45"/>
+      <c r="W149" s="45"/>
+      <c r="X149" s="45"/>
+      <c r="Y149" s="45"/>
+      <c r="Z149" s="45" t="s">
+        <v>305</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10196,7 +10248,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>

</xml_diff>

<commit_message>
fix VoverIplotter and DomeB meta stepping
</commit_message>
<xml_diff>
--- a/ivtools/sampledata/CeRAM_Depositions.xlsx
+++ b/ivtools/sampledata/CeRAM_Depositions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="314">
   <si>
     <t>wafer_number</t>
   </si>
@@ -938,6 +938,30 @@
   </si>
   <si>
     <t>contact test on new wafer with Pt from CS500 deposition tool</t>
+  </si>
+  <si>
+    <t>Murmeltier3</t>
+  </si>
+  <si>
+    <t>contact test on new wafer with Pt from CS500 deposition tool, sample taken out of vacuum for ~10 minutes</t>
+  </si>
+  <si>
+    <t>Zebra1</t>
+  </si>
+  <si>
+    <t>Zebra</t>
+  </si>
+  <si>
+    <t>first deposition on Au domeB; lift-of bad</t>
+  </si>
+  <si>
+    <t>Zebra2</t>
+  </si>
+  <si>
+    <t>first deposition on Au domeB; lift-of OK</t>
+  </si>
+  <si>
+    <t>W0044</t>
   </si>
 </sst>
 </file>
@@ -1583,7 +1607,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1681,6 +1705,9 @@
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="51" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2007,11 +2034,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z149"/>
+  <dimension ref="A1:Z152"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F149" sqref="F149"/>
+      <pane ySplit="9" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A151" sqref="A151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10234,6 +10261,148 @@
         <v>305</v>
       </c>
     </row>
+    <row r="150" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A150" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B150" s="87" t="s">
+        <v>300</v>
+      </c>
+      <c r="C150" s="45"/>
+      <c r="D150" s="46">
+        <v>43794</v>
+      </c>
+      <c r="E150" s="45" t="s">
+        <v>306</v>
+      </c>
+      <c r="F150" s="45" t="s">
+        <v>302</v>
+      </c>
+      <c r="G150" s="49">
+        <v>3</v>
+      </c>
+      <c r="H150" s="45"/>
+      <c r="I150" s="88" t="s">
+        <v>9</v>
+      </c>
+      <c r="J150" s="49">
+        <v>30</v>
+      </c>
+      <c r="K150" s="45"/>
+      <c r="L150" s="45"/>
+      <c r="M150" s="45"/>
+      <c r="N150" s="45"/>
+      <c r="O150" s="45"/>
+      <c r="P150" s="45"/>
+      <c r="Q150" s="45"/>
+      <c r="R150" s="45"/>
+      <c r="S150" s="45"/>
+      <c r="T150" s="45"/>
+      <c r="U150" s="45"/>
+      <c r="V150" s="45"/>
+      <c r="W150" s="45"/>
+      <c r="X150" s="45"/>
+      <c r="Y150" s="45"/>
+      <c r="Z150" s="45" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="151" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A151" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B151" s="89" t="s">
+        <v>313</v>
+      </c>
+      <c r="C151" s="16"/>
+      <c r="D151" s="17">
+        <v>43795</v>
+      </c>
+      <c r="E151" s="16" t="s">
+        <v>308</v>
+      </c>
+      <c r="F151" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="G151" s="90">
+        <v>1</v>
+      </c>
+      <c r="H151" s="16"/>
+      <c r="I151" s="91" t="s">
+        <v>29</v>
+      </c>
+      <c r="J151" s="90">
+        <v>30</v>
+      </c>
+      <c r="K151" s="16"/>
+      <c r="L151" s="16"/>
+      <c r="M151" s="16"/>
+      <c r="N151" s="16"/>
+      <c r="O151" s="16"/>
+      <c r="P151" s="16">
+        <v>298</v>
+      </c>
+      <c r="Q151" s="16"/>
+      <c r="R151" s="16"/>
+      <c r="S151" s="16"/>
+      <c r="T151" s="16"/>
+      <c r="U151" s="16"/>
+      <c r="V151" s="16"/>
+      <c r="W151" s="16"/>
+      <c r="X151" s="16"/>
+      <c r="Y151" s="16"/>
+      <c r="Z151" s="16" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="152" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A152" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="B152" s="89" t="s">
+        <v>313</v>
+      </c>
+      <c r="C152" s="16"/>
+      <c r="D152" s="17">
+        <v>43796</v>
+      </c>
+      <c r="E152" s="16" t="s">
+        <v>311</v>
+      </c>
+      <c r="F152" s="16" t="s">
+        <v>309</v>
+      </c>
+      <c r="G152" s="90">
+        <v>2</v>
+      </c>
+      <c r="H152" s="16"/>
+      <c r="I152" s="91" t="s">
+        <v>29</v>
+      </c>
+      <c r="J152" s="90">
+        <v>30</v>
+      </c>
+      <c r="K152" s="16"/>
+      <c r="L152" s="16"/>
+      <c r="M152" s="16"/>
+      <c r="N152" s="16"/>
+      <c r="O152" s="16"/>
+      <c r="P152" s="16">
+        <v>298</v>
+      </c>
+      <c r="Q152" s="16"/>
+      <c r="R152" s="16"/>
+      <c r="S152" s="16"/>
+      <c r="T152" s="16"/>
+      <c r="U152" s="16"/>
+      <c r="V152" s="16"/>
+      <c r="W152" s="16"/>
+      <c r="X152" s="16"/>
+      <c r="Y152" s="16"/>
+      <c r="Z152" s="16" t="s">
+        <v>312</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
made script for the conductivity measurements, should be reasonably functional
</commit_message>
<xml_diff>
--- a/ivtools/sampledata/CeRAM_Depositions.xlsx
+++ b/ivtools/sampledata/CeRAM_Depositions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\emrl\Pool\Projekte\HGST-CERAM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohr\py-ivtools\ivtools\sampledata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,12 @@
     <sheet name="deposition_plan" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1069" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="358">
   <si>
     <t>wafer_number</t>
   </si>
@@ -1082,6 +1082,18 @@
   </si>
   <si>
     <t>undoped NiO</t>
+  </si>
+  <si>
+    <t>NiO_CO2_lassen_1</t>
+  </si>
+  <si>
+    <t>NiO_CO2_lassen_2</t>
+  </si>
+  <si>
+    <t>Christdorn</t>
+  </si>
+  <si>
+    <t>NiO deposited with CO2 (20%)</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="59">
+  <fills count="60">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1566,6 +1578,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1727,7 +1745,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1831,50 +1849,53 @@
     <xf numFmtId="49" fontId="0" fillId="50" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="50" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="59" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="59" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="59" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1895,7 +1916,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2157,14 +2178,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z178"/>
+  <dimension ref="A1:Z180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D176" sqref="D176:D177"/>
+      <pane ySplit="9" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A179" sqref="A179"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -12210,6 +12231,114 @@
         <v>353</v>
       </c>
     </row>
+    <row r="179" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A179" s="95" t="s">
+        <v>83</v>
+      </c>
+      <c r="B179" s="95"/>
+      <c r="C179" s="95"/>
+      <c r="D179" s="96">
+        <v>44686</v>
+      </c>
+      <c r="E179" s="95" t="s">
+        <v>354</v>
+      </c>
+      <c r="F179" s="95" t="s">
+        <v>356</v>
+      </c>
+      <c r="G179" s="95">
+        <v>1</v>
+      </c>
+      <c r="H179" s="95"/>
+      <c r="I179" s="95" t="s">
+        <v>227</v>
+      </c>
+      <c r="J179" s="95">
+        <v>10</v>
+      </c>
+      <c r="K179" s="95"/>
+      <c r="L179" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="M179" s="95">
+        <v>10</v>
+      </c>
+      <c r="N179" s="95"/>
+      <c r="O179" s="95"/>
+      <c r="P179" s="95">
+        <v>673</v>
+      </c>
+      <c r="Q179" s="97">
+        <v>17</v>
+      </c>
+      <c r="R179" s="95">
+        <v>76.5</v>
+      </c>
+      <c r="S179" s="95"/>
+      <c r="T179" s="95"/>
+      <c r="U179" s="95"/>
+      <c r="V179" s="95"/>
+      <c r="W179" s="95"/>
+      <c r="X179" s="95"/>
+      <c r="Y179" s="95"/>
+      <c r="Z179" s="95" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="180" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A180" s="95" t="s">
+        <v>83</v>
+      </c>
+      <c r="B180" s="95"/>
+      <c r="C180" s="95"/>
+      <c r="D180" s="96">
+        <v>44686</v>
+      </c>
+      <c r="E180" s="95" t="s">
+        <v>355</v>
+      </c>
+      <c r="F180" s="95" t="s">
+        <v>356</v>
+      </c>
+      <c r="G180" s="95">
+        <v>2</v>
+      </c>
+      <c r="H180" s="95"/>
+      <c r="I180" s="95" t="s">
+        <v>227</v>
+      </c>
+      <c r="J180" s="95">
+        <v>10</v>
+      </c>
+      <c r="K180" s="95"/>
+      <c r="L180" s="95" t="s">
+        <v>9</v>
+      </c>
+      <c r="M180" s="95">
+        <v>10</v>
+      </c>
+      <c r="N180" s="95"/>
+      <c r="O180" s="95"/>
+      <c r="P180" s="95">
+        <v>673</v>
+      </c>
+      <c r="Q180" s="97">
+        <v>17</v>
+      </c>
+      <c r="R180" s="95">
+        <v>76.5</v>
+      </c>
+      <c r="S180" s="95"/>
+      <c r="T180" s="95"/>
+      <c r="U180" s="95"/>
+      <c r="V180" s="95"/>
+      <c r="W180" s="95"/>
+      <c r="X180" s="95"/>
+      <c r="Y180" s="95"/>
+      <c r="Z180" s="95" t="s">
+        <v>357</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -12224,7 +12353,7 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>

</xml_diff>